<commit_message>
excel template: remove a comment
</commit_message>
<xml_diff>
--- a/src/main/dart/web/LCI-Database_Data-collection_Crop_v1.xlsx
+++ b/src/main/dart/web/LCI-Database_Data-collection_Crop_v1.xlsx
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2366" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2365" uniqueCount="992">
   <si>
     <t>Country</t>
   </si>
@@ -6109,6 +6109,18 @@
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6120,18 +6132,6 @@
     </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -8995,25 +8995,25 @@
     </row>
     <row r="5" spans="1:9" s="160" customFormat="1" ht="54.75" customHeight="1">
       <c r="A5" s="159"/>
-      <c r="B5" s="317"/>
-      <c r="C5" s="317"/>
-      <c r="D5" s="317"/>
-      <c r="E5" s="317"/>
-      <c r="F5" s="317"/>
-      <c r="G5" s="317"/>
+      <c r="B5" s="313"/>
+      <c r="C5" s="313"/>
+      <c r="D5" s="313"/>
+      <c r="E5" s="313"/>
+      <c r="F5" s="313"/>
+      <c r="G5" s="313"/>
       <c r="H5" s="156"/>
       <c r="I5" s="156"/>
     </row>
     <row r="6" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A6" s="154"/>
-      <c r="B6" s="318" t="s">
+      <c r="B6" s="314" t="s">
         <v>791</v>
       </c>
-      <c r="C6" s="318"/>
-      <c r="D6" s="318"/>
-      <c r="E6" s="318"/>
-      <c r="F6" s="318"/>
-      <c r="G6" s="318"/>
+      <c r="C6" s="314"/>
+      <c r="D6" s="314"/>
+      <c r="E6" s="314"/>
+      <c r="F6" s="314"/>
+      <c r="G6" s="314"/>
       <c r="H6" s="156"/>
       <c r="I6" s="156"/>
     </row>
@@ -9030,14 +9030,14 @@
     </row>
     <row r="8" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A8" s="154"/>
-      <c r="B8" s="319" t="s">
+      <c r="B8" s="315" t="s">
         <v>766</v>
       </c>
-      <c r="C8" s="319"/>
-      <c r="D8" s="319"/>
-      <c r="E8" s="319"/>
-      <c r="F8" s="319"/>
-      <c r="G8" s="319"/>
+      <c r="C8" s="315"/>
+      <c r="D8" s="315"/>
+      <c r="E8" s="315"/>
+      <c r="F8" s="315"/>
+      <c r="G8" s="315"/>
       <c r="H8" s="161"/>
       <c r="I8" s="156"/>
     </row>
@@ -9054,14 +9054,14 @@
     </row>
     <row r="10" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A10" s="154"/>
-      <c r="B10" s="320" t="s">
+      <c r="B10" s="316" t="s">
         <v>831</v>
       </c>
-      <c r="C10" s="320"/>
-      <c r="D10" s="320"/>
-      <c r="E10" s="320"/>
-      <c r="F10" s="320"/>
-      <c r="G10" s="320"/>
+      <c r="C10" s="316"/>
+      <c r="D10" s="316"/>
+      <c r="E10" s="316"/>
+      <c r="F10" s="316"/>
+      <c r="G10" s="316"/>
       <c r="H10" s="156"/>
       <c r="I10" s="156"/>
     </row>
@@ -9069,10 +9069,10 @@
       <c r="A11" s="154"/>
       <c r="B11" s="173"/>
       <c r="C11" s="173"/>
-      <c r="D11" s="320"/>
-      <c r="E11" s="320"/>
-      <c r="F11" s="320"/>
-      <c r="G11" s="320"/>
+      <c r="D11" s="316"/>
+      <c r="E11" s="316"/>
+      <c r="F11" s="316"/>
+      <c r="G11" s="316"/>
       <c r="H11" s="156"/>
       <c r="I11" s="156"/>
     </row>
@@ -9145,23 +9145,23 @@
     </row>
     <row r="17" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A17" s="154"/>
-      <c r="B17" s="314" t="s">
+      <c r="B17" s="318" t="s">
         <v>769</v>
       </c>
-      <c r="C17" s="314"/>
-      <c r="D17" s="314"/>
-      <c r="E17" s="314"/>
-      <c r="F17" s="314"/>
-      <c r="G17" s="314"/>
+      <c r="C17" s="318"/>
+      <c r="D17" s="318"/>
+      <c r="E17" s="318"/>
+      <c r="F17" s="318"/>
+      <c r="G17" s="318"/>
       <c r="H17" s="161"/>
       <c r="I17" s="156"/>
     </row>
     <row r="18" spans="1:9" s="160" customFormat="1">
       <c r="A18" s="159"/>
-      <c r="B18" s="315" t="s">
+      <c r="B18" s="319" t="s">
         <v>770</v>
       </c>
-      <c r="C18" s="315"/>
+      <c r="C18" s="319"/>
       <c r="D18" s="180" t="s">
         <v>771</v>
       </c>
@@ -9179,10 +9179,10 @@
     </row>
     <row r="19" spans="1:9" s="160" customFormat="1">
       <c r="A19" s="159"/>
-      <c r="B19" s="316" t="s">
+      <c r="B19" s="320" t="s">
         <v>775</v>
       </c>
-      <c r="C19" s="316"/>
+      <c r="C19" s="320"/>
       <c r="D19" s="166" t="s">
         <v>776</v>
       </c>
@@ -9221,10 +9221,10 @@
     </row>
     <row r="21" spans="1:9" s="160" customFormat="1">
       <c r="A21" s="159"/>
-      <c r="B21" s="313" t="s">
+      <c r="B21" s="317" t="s">
         <v>778</v>
       </c>
-      <c r="C21" s="313"/>
+      <c r="C21" s="317"/>
       <c r="D21" s="167" t="s">
         <v>779</v>
       </c>
@@ -9242,10 +9242,10 @@
     </row>
     <row r="22" spans="1:9" s="160" customFormat="1" ht="25.5">
       <c r="A22" s="159"/>
-      <c r="B22" s="313" t="s">
+      <c r="B22" s="317" t="s">
         <v>782</v>
       </c>
-      <c r="C22" s="313"/>
+      <c r="C22" s="317"/>
       <c r="D22" s="167" t="s">
         <v>783</v>
       </c>
@@ -9359,12 +9359,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="D11:G11"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="B21:C21"/>
@@ -9373,6 +9367,12 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
@@ -13561,9 +13561,9 @@
   <dimension ref="A1:AB256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B35" sqref="B35"/>
-      <selection pane="bottomLeft" sqref="A1:A1048576"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -14991,9 +14991,7 @@
       <c r="E86" s="108" t="s">
         <v>100</v>
       </c>
-      <c r="F86" s="31" t="s">
-        <v>717</v>
-      </c>
+      <c r="F86" s="31"/>
       <c r="G86" s="38"/>
       <c r="H86" s="18"/>
     </row>

</xml_diff>

<commit_message>
ALCIG-30: Fix template (fix ecopsold_location, TIR)
</commit_message>
<xml_diff>
--- a/src/main/dart/web/LCI-Database_Data-collection_Crop_v1.xlsx
+++ b/src/main/dart/web/LCI-Database_Data-collection_Crop_v1.xlsx
@@ -2814,9 +2814,6 @@
     <t>Geographical representativeness (GR)</t>
   </si>
   <si>
-    <t>Time-related representativeness (TIR)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Completeness (C) </t>
   </si>
   <si>
@@ -2975,9 +2972,6 @@
     <t>ecospold_name</t>
   </si>
   <si>
-    <t>ecopsold_location</t>
-  </si>
-  <si>
     <t>ecospold_infra_process</t>
   </si>
   <si>
@@ -3315,6 +3309,12 @@
   </si>
   <si>
     <t>Triazamate</t>
+  </si>
+  <si>
+    <t>ecospold_location</t>
+  </si>
+  <si>
+    <t>Time-related representativeness (TiR)</t>
   </si>
 </sst>
 </file>
@@ -5927,9 +5927,24 @@
     <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5942,18 +5957,6 @@
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5968,9 +5971,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="613">
@@ -8928,25 +8928,25 @@
     </row>
     <row r="5" spans="1:9" s="160" customFormat="1" ht="54.75" customHeight="1">
       <c r="A5" s="159"/>
-      <c r="B5" s="261"/>
-      <c r="C5" s="261"/>
-      <c r="D5" s="261"/>
-      <c r="E5" s="261"/>
-      <c r="F5" s="261"/>
-      <c r="G5" s="261"/>
+      <c r="B5" s="258"/>
+      <c r="C5" s="258"/>
+      <c r="D5" s="258"/>
+      <c r="E5" s="258"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="258"/>
       <c r="H5" s="156"/>
       <c r="I5" s="156"/>
     </row>
     <row r="6" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A6" s="154"/>
-      <c r="B6" s="262" t="s">
+      <c r="B6" s="259" t="s">
         <v>734</v>
       </c>
-      <c r="C6" s="262"/>
-      <c r="D6" s="262"/>
-      <c r="E6" s="262"/>
-      <c r="F6" s="262"/>
-      <c r="G6" s="262"/>
+      <c r="C6" s="259"/>
+      <c r="D6" s="259"/>
+      <c r="E6" s="259"/>
+      <c r="F6" s="259"/>
+      <c r="G6" s="259"/>
       <c r="H6" s="156"/>
       <c r="I6" s="156"/>
     </row>
@@ -8963,14 +8963,14 @@
     </row>
     <row r="8" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A8" s="154"/>
-      <c r="B8" s="263" t="s">
+      <c r="B8" s="260" t="s">
         <v>709</v>
       </c>
-      <c r="C8" s="263"/>
-      <c r="D8" s="263"/>
-      <c r="E8" s="263"/>
-      <c r="F8" s="263"/>
-      <c r="G8" s="263"/>
+      <c r="C8" s="260"/>
+      <c r="D8" s="260"/>
+      <c r="E8" s="260"/>
+      <c r="F8" s="260"/>
+      <c r="G8" s="260"/>
       <c r="H8" s="161"/>
       <c r="I8" s="156"/>
     </row>
@@ -8987,14 +8987,14 @@
     </row>
     <row r="10" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A10" s="154"/>
-      <c r="B10" s="264" t="s">
+      <c r="B10" s="261" t="s">
         <v>774</v>
       </c>
-      <c r="C10" s="264"/>
-      <c r="D10" s="264"/>
-      <c r="E10" s="264"/>
-      <c r="F10" s="264"/>
-      <c r="G10" s="264"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
+      <c r="G10" s="261"/>
       <c r="H10" s="156"/>
       <c r="I10" s="156"/>
     </row>
@@ -9002,10 +9002,10 @@
       <c r="A11" s="154"/>
       <c r="B11" s="173"/>
       <c r="C11" s="173"/>
-      <c r="D11" s="264"/>
-      <c r="E11" s="264"/>
-      <c r="F11" s="264"/>
-      <c r="G11" s="264"/>
+      <c r="D11" s="261"/>
+      <c r="E11" s="261"/>
+      <c r="F11" s="261"/>
+      <c r="G11" s="261"/>
       <c r="H11" s="156"/>
       <c r="I11" s="156"/>
     </row>
@@ -9015,12 +9015,12 @@
         <v>710</v>
       </c>
       <c r="C12" s="174"/>
-      <c r="D12" s="256" t="s">
+      <c r="D12" s="257" t="s">
         <v>711</v>
       </c>
-      <c r="E12" s="256"/>
-      <c r="F12" s="256"/>
-      <c r="G12" s="256"/>
+      <c r="E12" s="257"/>
+      <c r="F12" s="257"/>
+      <c r="G12" s="257"/>
       <c r="H12" s="156"/>
       <c r="I12" s="156"/>
     </row>
@@ -9030,12 +9030,12 @@
         <v>739</v>
       </c>
       <c r="C13" s="174"/>
-      <c r="D13" s="256" t="s">
+      <c r="D13" s="257" t="s">
         <v>741</v>
       </c>
-      <c r="E13" s="256"/>
-      <c r="F13" s="256"/>
-      <c r="G13" s="256"/>
+      <c r="E13" s="257"/>
+      <c r="F13" s="257"/>
+      <c r="G13" s="257"/>
       <c r="H13" s="156"/>
       <c r="I13" s="156"/>
     </row>
@@ -9045,12 +9045,12 @@
         <v>740</v>
       </c>
       <c r="C14" s="174"/>
-      <c r="D14" s="256" t="s">
+      <c r="D14" s="257" t="s">
         <v>742</v>
       </c>
-      <c r="E14" s="256"/>
-      <c r="F14" s="256"/>
-      <c r="G14" s="256"/>
+      <c r="E14" s="257"/>
+      <c r="F14" s="257"/>
+      <c r="G14" s="257"/>
       <c r="H14" s="156"/>
       <c r="I14" s="156"/>
     </row>
@@ -9058,10 +9058,10 @@
       <c r="A15" s="154"/>
       <c r="B15" s="175"/>
       <c r="C15" s="174"/>
-      <c r="D15" s="256"/>
-      <c r="E15" s="256"/>
-      <c r="F15" s="256"/>
-      <c r="G15" s="256"/>
+      <c r="D15" s="257"/>
+      <c r="E15" s="257"/>
+      <c r="F15" s="257"/>
+      <c r="G15" s="257"/>
       <c r="H15" s="156"/>
       <c r="I15" s="156"/>
     </row>
@@ -9078,23 +9078,23 @@
     </row>
     <row r="17" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A17" s="154"/>
-      <c r="B17" s="258" t="s">
+      <c r="B17" s="263" t="s">
         <v>712</v>
       </c>
-      <c r="C17" s="258"/>
-      <c r="D17" s="258"/>
-      <c r="E17" s="258"/>
-      <c r="F17" s="258"/>
-      <c r="G17" s="258"/>
+      <c r="C17" s="263"/>
+      <c r="D17" s="263"/>
+      <c r="E17" s="263"/>
+      <c r="F17" s="263"/>
+      <c r="G17" s="263"/>
       <c r="H17" s="161"/>
       <c r="I17" s="156"/>
     </row>
     <row r="18" spans="1:9" s="160" customFormat="1">
       <c r="A18" s="159"/>
-      <c r="B18" s="259" t="s">
+      <c r="B18" s="264" t="s">
         <v>713</v>
       </c>
-      <c r="C18" s="259"/>
+      <c r="C18" s="264"/>
       <c r="D18" s="180" t="s">
         <v>714</v>
       </c>
@@ -9112,10 +9112,10 @@
     </row>
     <row r="19" spans="1:9" s="160" customFormat="1">
       <c r="A19" s="159"/>
-      <c r="B19" s="260" t="s">
+      <c r="B19" s="265" t="s">
         <v>718</v>
       </c>
-      <c r="C19" s="260"/>
+      <c r="C19" s="265"/>
       <c r="D19" s="166" t="s">
         <v>719</v>
       </c>
@@ -9154,10 +9154,10 @@
     </row>
     <row r="21" spans="1:9" s="160" customFormat="1">
       <c r="A21" s="159"/>
-      <c r="B21" s="257" t="s">
+      <c r="B21" s="262" t="s">
         <v>721</v>
       </c>
-      <c r="C21" s="257"/>
+      <c r="C21" s="262"/>
       <c r="D21" s="167" t="s">
         <v>722</v>
       </c>
@@ -9175,10 +9175,10 @@
     </row>
     <row r="22" spans="1:9" s="160" customFormat="1" ht="25.5">
       <c r="A22" s="159"/>
-      <c r="B22" s="257" t="s">
+      <c r="B22" s="262" t="s">
         <v>725</v>
       </c>
-      <c r="C22" s="257"/>
+      <c r="C22" s="262"/>
       <c r="D22" s="167" t="s">
         <v>726</v>
       </c>
@@ -9292,12 +9292,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="D11:G11"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="B21:C21"/>
@@ -9306,6 +9300,12 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
@@ -9331,10 +9331,10 @@
   </sheetPr>
   <dimension ref="A1:Z245"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B35" sqref="B35"/>
-      <selection pane="bottomLeft" activeCell="A204" sqref="A204:XFD204"/>
+      <selection pane="bottomLeft" activeCell="E68" sqref="E68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -9364,12 +9364,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="11" customFormat="1" ht="90" customHeight="1">
-      <c r="B2" s="265" t="s">
+      <c r="B2" s="266" t="s">
         <v>743</v>
       </c>
-      <c r="C2" s="265"/>
-      <c r="D2" s="265"/>
-      <c r="E2" s="265"/>
+      <c r="C2" s="266"/>
+      <c r="D2" s="266"/>
+      <c r="E2" s="266"/>
       <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" s="11" customFormat="1" ht="15.95" customHeight="1">
@@ -9384,10 +9384,10 @@
       <c r="C4" s="196" t="s">
         <v>744</v>
       </c>
-      <c r="D4" s="266" t="s">
+      <c r="D4" s="267" t="s">
         <v>776</v>
       </c>
-      <c r="E4" s="266"/>
+      <c r="E4" s="267"/>
       <c r="F4" s="63"/>
     </row>
     <row r="5" spans="1:6" s="11" customFormat="1" ht="30.95" customHeight="1">
@@ -9395,10 +9395,10 @@
       <c r="C5" s="196" t="s">
         <v>745</v>
       </c>
-      <c r="D5" s="267" t="s">
+      <c r="D5" s="268" t="s">
         <v>775</v>
       </c>
-      <c r="E5" s="267"/>
+      <c r="E5" s="268"/>
       <c r="F5" s="63"/>
     </row>
     <row r="6" spans="1:6" ht="8.1" customHeight="1">
@@ -10271,7 +10271,7 @@
     <row r="66" spans="1:6" outlineLevel="1">
       <c r="A66" s="153"/>
       <c r="C66" s="19" t="s">
-        <v>816</v>
+        <v>975</v>
       </c>
       <c r="D66" s="25" t="s">
         <v>814</v>
@@ -10284,7 +10284,7 @@
     <row r="67" spans="1:6" outlineLevel="1">
       <c r="A67" s="153"/>
       <c r="C67" s="19" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>814</v>
@@ -10297,7 +10297,7 @@
     <row r="68" spans="1:6" outlineLevel="1">
       <c r="A68" s="153"/>
       <c r="C68" s="19" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>814</v>
@@ -10310,7 +10310,7 @@
     <row r="69" spans="1:6" outlineLevel="1">
       <c r="A69" s="153"/>
       <c r="C69" s="19" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>814</v>
@@ -10361,7 +10361,7 @@
         <v>248</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>22</v>
@@ -10401,7 +10401,7 @@
         <v>250</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D76" s="27" t="s">
         <v>101</v>
@@ -10752,7 +10752,7 @@
         <v>32</v>
       </c>
       <c r="E100" s="214" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F100" s="64"/>
     </row>
@@ -10835,7 +10835,7 @@
         <v>291</v>
       </c>
       <c r="C106" s="46" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D106" s="23" t="s">
         <v>22</v>
@@ -10940,7 +10940,7 @@
         <v>288</v>
       </c>
       <c r="C113" s="46" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D113" s="23" t="s">
         <v>22</v>
@@ -10986,7 +10986,7 @@
         <v>301</v>
       </c>
       <c r="C116" s="46" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D116" s="23" t="s">
         <v>22</v>
@@ -11001,7 +11001,7 @@
         <v>300</v>
       </c>
       <c r="C117" s="46" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D117" s="23" t="s">
         <v>22</v>
@@ -11016,7 +11016,7 @@
         <v>303</v>
       </c>
       <c r="C118" s="46" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D118" s="23" t="s">
         <v>22</v>
@@ -11031,7 +11031,7 @@
         <v>299</v>
       </c>
       <c r="C119" s="46" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D119" s="23" t="s">
         <v>22</v>
@@ -11046,7 +11046,7 @@
         <v>302</v>
       </c>
       <c r="C120" s="46" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D120" s="23" t="s">
         <v>22</v>
@@ -11061,7 +11061,7 @@
         <v>298</v>
       </c>
       <c r="C121" s="46" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D121" s="23" t="s">
         <v>22</v>
@@ -11076,7 +11076,7 @@
         <v>297</v>
       </c>
       <c r="C122" s="46" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D122" s="23" t="s">
         <v>22</v>
@@ -11580,7 +11580,7 @@
         <v>53</v>
       </c>
       <c r="E156" s="222" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F156" s="64"/>
     </row>
@@ -11893,7 +11893,7 @@
       </c>
       <c r="B181" s="7"/>
       <c r="C181" s="5" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D181" s="7" t="s">
         <v>27</v>
@@ -11927,7 +11927,7 @@
       </c>
       <c r="B183" s="12"/>
       <c r="C183" s="29" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D183" s="12" t="s">
         <v>27</v>
@@ -12000,7 +12000,7 @@
       </c>
       <c r="B187" s="12"/>
       <c r="C187" s="29" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D187" s="12" t="s">
         <v>27</v>
@@ -12073,7 +12073,7 @@
       </c>
       <c r="B191" s="12"/>
       <c r="C191" s="134" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D191" s="139" t="s">
         <v>27</v>
@@ -12146,7 +12146,7 @@
       </c>
       <c r="B195" s="12"/>
       <c r="C195" s="29" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D195" s="12" t="s">
         <v>27</v>
@@ -12220,7 +12220,7 @@
       </c>
       <c r="B199" s="12"/>
       <c r="C199" s="134" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D199" s="12" t="s">
         <v>27</v>
@@ -12294,7 +12294,7 @@
       </c>
       <c r="B203" s="12"/>
       <c r="C203" s="134" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D203" s="139" t="s">
         <v>27</v>
@@ -12351,7 +12351,7 @@
       </c>
       <c r="B206" s="120"/>
       <c r="C206" s="122" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D206" s="123" t="s">
         <v>8</v>
@@ -12411,7 +12411,7 @@
       </c>
       <c r="B209" s="12"/>
       <c r="C209" s="26" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D209" s="7" t="s">
         <v>143</v>
@@ -12432,7 +12432,7 @@
       </c>
       <c r="B210" s="12"/>
       <c r="C210" s="26" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D210" s="7" t="s">
         <v>143</v>
@@ -12867,7 +12867,7 @@
     <row r="223" spans="1:26" s="198" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B223" s="199"/>
       <c r="C223" s="204" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D223" s="228" t="s">
         <v>8</v>
@@ -12930,7 +12930,7 @@
       </c>
       <c r="B226" s="12"/>
       <c r="C226" s="26" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D226" s="7" t="s">
         <v>33</v>
@@ -12983,7 +12983,7 @@
         <v>27</v>
       </c>
       <c r="E229" s="223" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F229" s="64"/>
     </row>
@@ -13131,7 +13131,7 @@
     <row r="239" spans="1:26" s="86" customFormat="1" ht="35.1" customHeight="1">
       <c r="B239" s="88"/>
       <c r="C239" s="124" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D239" s="125" t="s">
         <v>8</v>
@@ -13229,7 +13229,7 @@
       </c>
       <c r="B243" s="12"/>
       <c r="C243" s="26" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D243" s="86" t="s">
         <v>33</v>
@@ -13250,7 +13250,7 @@
       </c>
       <c r="B244" s="12"/>
       <c r="C244" s="26" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D244" s="86" t="s">
         <v>33</v>
@@ -13271,10 +13271,10 @@
       </c>
       <c r="B245" s="12"/>
       <c r="C245" s="26" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D245" s="86" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E245" s="223" t="s">
         <v>100</v>
@@ -13385,7 +13385,7 @@
   </sheetPr>
   <dimension ref="A1:AB245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B35" sqref="B35"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
@@ -13393,7 +13393,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="4" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="12" customWidth="1"/>
     <col min="3" max="3" width="51.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" style="8" customWidth="1"/>
@@ -13426,14 +13426,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="78" customHeight="1">
-      <c r="B2" s="265" t="s">
+      <c r="B2" s="266" t="s">
         <v>743</v>
       </c>
-      <c r="C2" s="265"/>
-      <c r="D2" s="265"/>
-      <c r="E2" s="265"/>
-      <c r="F2" s="265"/>
-      <c r="G2" s="265"/>
+      <c r="C2" s="266"/>
+      <c r="D2" s="266"/>
+      <c r="E2" s="266"/>
+      <c r="F2" s="266"/>
+      <c r="G2" s="266"/>
       <c r="H2" s="62"/>
     </row>
     <row r="3" spans="1:8" s="11" customFormat="1" ht="15.95" customHeight="1">
@@ -13447,34 +13447,34 @@
     </row>
     <row r="4" spans="1:8" ht="21">
       <c r="A4" s="153" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B4" s="188"/>
       <c r="C4" s="192" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="D4" s="190" t="s">
         <v>661</v>
       </c>
-      <c r="E4" s="268"/>
-      <c r="F4" s="268"/>
-      <c r="G4" s="268"/>
+      <c r="E4" s="269"/>
+      <c r="F4" s="269"/>
+      <c r="G4" s="269"/>
       <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:8" ht="21">
       <c r="A5" s="153" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B5" s="189"/>
       <c r="C5" s="193" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="D5" s="191" t="s">
         <v>662</v>
       </c>
-      <c r="E5" s="269"/>
-      <c r="F5" s="269"/>
-      <c r="G5" s="269"/>
+      <c r="E5" s="270"/>
+      <c r="F5" s="270"/>
+      <c r="G5" s="270"/>
       <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:8" ht="8.1" customHeight="1">
@@ -13613,7 +13613,7 @@
     </row>
     <row r="15" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A15" s="254" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>663</v>
@@ -13630,7 +13630,7 @@
     </row>
     <row r="16" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A16" s="153" t="s">
-        <v>862</v>
+        <v>974</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>664</v>
@@ -13647,7 +13647,7 @@
     </row>
     <row r="17" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A17" s="153" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>665</v>
@@ -13664,7 +13664,7 @@
     </row>
     <row r="18" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A18" s="254" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>8</v>
@@ -13681,7 +13681,7 @@
     </row>
     <row r="19" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A19" s="153" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>666</v>
@@ -13698,7 +13698,7 @@
     </row>
     <row r="20" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A20" s="153" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>667</v>
@@ -13715,7 +13715,7 @@
     </row>
     <row r="21" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A21" s="153" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>668</v>
@@ -13732,7 +13732,7 @@
     </row>
     <row r="22" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A22" s="153" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>669</v>
@@ -13749,7 +13749,7 @@
     </row>
     <row r="23" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A23" s="153" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>670</v>
@@ -13766,7 +13766,7 @@
     </row>
     <row r="24" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A24" s="153" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
       <c r="C24" s="19" t="s">
         <v>671</v>
@@ -13783,7 +13783,7 @@
     </row>
     <row r="25" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A25" s="153" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
       <c r="C25" s="19" t="s">
         <v>672</v>
@@ -13800,7 +13800,7 @@
     </row>
     <row r="26" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A26" s="153" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
       <c r="C26" s="19" t="s">
         <v>673</v>
@@ -13817,7 +13817,7 @@
     </row>
     <row r="27" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A27" s="153" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
       <c r="C27" s="19" t="s">
         <v>674</v>
@@ -13834,7 +13834,7 @@
     </row>
     <row r="28" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A28" s="153" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
       <c r="C28" s="19" t="s">
         <v>675</v>
@@ -13851,7 +13851,7 @@
     </row>
     <row r="29" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A29" s="153" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
       <c r="C29" s="19" t="s">
         <v>676</v>
@@ -13868,7 +13868,7 @@
     </row>
     <row r="30" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A30" s="153" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
       <c r="C30" s="19" t="s">
         <v>677</v>
@@ -13885,7 +13885,7 @@
     </row>
     <row r="31" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A31" s="153" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
       <c r="C31" s="19" t="s">
         <v>678</v>
@@ -13902,7 +13902,7 @@
     </row>
     <row r="32" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A32" s="153" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
       <c r="C32" s="19" t="s">
         <v>679</v>
@@ -13919,7 +13919,7 @@
     </row>
     <row r="33" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A33" s="153" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
       <c r="C33" s="19" t="s">
         <v>680</v>
@@ -13936,7 +13936,7 @@
     </row>
     <row r="34" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A34" s="153" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
       <c r="C34" s="19" t="s">
         <v>681</v>
@@ -13953,7 +13953,7 @@
     </row>
     <row r="35" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A35" s="153" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
       <c r="C35" s="19" t="s">
         <v>682</v>
@@ -13970,7 +13970,7 @@
     </row>
     <row r="36" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A36" s="153" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
       <c r="C36" s="19" t="s">
         <v>683</v>
@@ -13987,7 +13987,7 @@
     </row>
     <row r="37" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A37" s="153" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
       <c r="C37" s="19" t="s">
         <v>684</v>
@@ -14004,7 +14004,7 @@
     </row>
     <row r="38" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A38" s="254" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
       <c r="C38" s="19" t="s">
         <v>685</v>
@@ -14021,7 +14021,7 @@
     </row>
     <row r="39" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A39" s="153" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
       <c r="C39" s="19" t="s">
         <v>686</v>
@@ -14038,7 +14038,7 @@
     </row>
     <row r="40" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A40" s="153" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
       <c r="C40" s="19" t="s">
         <v>687</v>
@@ -14055,7 +14055,7 @@
     </row>
     <row r="41" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A41" s="153" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
       <c r="C41" s="19" t="s">
         <v>688</v>
@@ -14072,7 +14072,7 @@
     </row>
     <row r="42" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A42" s="153" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
       <c r="C42" s="19" t="s">
         <v>689</v>
@@ -14089,7 +14089,7 @@
     </row>
     <row r="43" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A43" s="153" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="C43" s="19" t="s">
         <v>690</v>
@@ -14106,7 +14106,7 @@
     </row>
     <row r="44" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A44" s="153" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="C44" s="19" t="s">
         <v>690</v>
@@ -14123,7 +14123,7 @@
     </row>
     <row r="45" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A45" s="153" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="C45" s="19" t="s">
         <v>691</v>
@@ -14140,7 +14140,7 @@
     </row>
     <row r="46" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A46" s="153" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="C46" s="19" t="s">
         <v>692</v>
@@ -14157,7 +14157,7 @@
     </row>
     <row r="47" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A47" s="153" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="C47" s="19" t="s">
         <v>693</v>
@@ -14174,7 +14174,7 @@
     </row>
     <row r="48" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A48" s="153" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="C48" s="19" t="s">
         <v>694</v>
@@ -14191,7 +14191,7 @@
     </row>
     <row r="49" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A49" s="153" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="C49" s="19" t="s">
         <v>695</v>
@@ -14208,7 +14208,7 @@
     </row>
     <row r="50" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A50" s="153" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="C50" s="19" t="s">
         <v>696</v>
@@ -14225,7 +14225,7 @@
     </row>
     <row r="51" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A51" s="153" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="C51" s="19" t="s">
         <v>696</v>
@@ -14242,7 +14242,7 @@
     </row>
     <row r="52" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A52" s="153" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="C52" s="19" t="s">
         <v>697</v>
@@ -14259,7 +14259,7 @@
     </row>
     <row r="53" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A53" s="153" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>698</v>
@@ -14276,7 +14276,7 @@
     </row>
     <row r="54" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A54" s="153" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="C54" s="19" t="s">
         <v>699</v>
@@ -14293,7 +14293,7 @@
     </row>
     <row r="55" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A55" s="153" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="C55" s="19" t="s">
         <v>700</v>
@@ -14310,7 +14310,7 @@
     </row>
     <row r="56" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A56" s="153" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="C56" s="19" t="s">
         <v>701</v>
@@ -14327,7 +14327,7 @@
     </row>
     <row r="57" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A57" s="153" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="C57" s="19" t="s">
         <v>702</v>
@@ -14344,7 +14344,7 @@
     </row>
     <row r="58" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A58" s="153" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="C58" s="19" t="s">
         <v>703</v>
@@ -14361,7 +14361,7 @@
     </row>
     <row r="59" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A59" s="153" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="C59" s="19" t="s">
         <v>704</v>
@@ -14378,7 +14378,7 @@
     </row>
     <row r="60" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A60" s="153" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="C60" s="19" t="s">
         <v>705</v>
@@ -14395,7 +14395,7 @@
     </row>
     <row r="61" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A61" s="153" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="C61" s="19" t="s">
         <v>706</v>
@@ -14412,7 +14412,7 @@
     </row>
     <row r="62" spans="1:8" hidden="1" outlineLevel="2">
       <c r="A62" s="153" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="C62" s="19" t="s">
         <v>707</v>
@@ -14440,7 +14440,7 @@
     </row>
     <row r="64" spans="1:8" outlineLevel="1">
       <c r="A64" s="153" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="C64" s="19" t="s">
         <v>813</v>
@@ -14457,7 +14457,7 @@
     </row>
     <row r="65" spans="1:8" outlineLevel="1">
       <c r="A65" s="153" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="C65" s="19" t="s">
         <v>815</v>
@@ -14474,10 +14474,10 @@
     </row>
     <row r="66" spans="1:8" outlineLevel="1">
       <c r="A66" s="153" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>816</v>
+        <v>975</v>
       </c>
       <c r="D66" s="25" t="s">
         <v>814</v>
@@ -14491,10 +14491,10 @@
     </row>
     <row r="67" spans="1:8" outlineLevel="1">
       <c r="A67" s="153" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D67" s="25" t="s">
         <v>814</v>
@@ -14508,10 +14508,10 @@
     </row>
     <row r="68" spans="1:8" outlineLevel="1">
       <c r="A68" s="153" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D68" s="25" t="s">
         <v>814</v>
@@ -14525,10 +14525,10 @@
     </row>
     <row r="69" spans="1:8" outlineLevel="1">
       <c r="A69" s="153" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="C69" s="19" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="D69" s="25" t="s">
         <v>814</v>
@@ -14591,7 +14591,7 @@
         <v>248</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>22</v>
@@ -15142,7 +15142,7 @@
         <v>291</v>
       </c>
       <c r="C106" s="46" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D106" s="39" t="s">
         <v>22</v>
@@ -15261,7 +15261,7 @@
         <v>288</v>
       </c>
       <c r="C113" s="46" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D113" s="39" t="s">
         <v>22</v>
@@ -15314,7 +15314,7 @@
         <v>301</v>
       </c>
       <c r="C116" s="238" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D116" s="39" t="s">
         <v>22</v>
@@ -15331,7 +15331,7 @@
         <v>300</v>
       </c>
       <c r="C117" s="238" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D117" s="39" t="s">
         <v>22</v>
@@ -15348,7 +15348,7 @@
         <v>303</v>
       </c>
       <c r="C118" s="46" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D118" s="39" t="s">
         <v>22</v>
@@ -15365,7 +15365,7 @@
         <v>299</v>
       </c>
       <c r="C119" s="238" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D119" s="39" t="s">
         <v>22</v>
@@ -15382,7 +15382,7 @@
         <v>302</v>
       </c>
       <c r="C120" s="46" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D120" s="39" t="s">
         <v>22</v>
@@ -15399,7 +15399,7 @@
         <v>298</v>
       </c>
       <c r="C121" s="46" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D121" s="39" t="s">
         <v>22</v>
@@ -15416,7 +15416,7 @@
         <v>297</v>
       </c>
       <c r="C122" s="46" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D122" s="39" t="s">
         <v>22</v>
@@ -15708,7 +15708,7 @@
     </row>
     <row r="139" spans="1:8" outlineLevel="1">
       <c r="A139" s="250" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C139" s="236" t="s">
         <v>798</v>
@@ -15742,7 +15742,7 @@
     </row>
     <row r="141" spans="1:8" outlineLevel="1">
       <c r="A141" s="250" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C141" s="236" t="s">
         <v>800</v>
@@ -16397,7 +16397,7 @@
       </c>
       <c r="B181" s="7"/>
       <c r="C181" s="5" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D181" s="7" t="s">
         <v>27</v>
@@ -16439,7 +16439,7 @@
       </c>
       <c r="B183" s="12"/>
       <c r="C183" s="29" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D183" s="12" t="s">
         <v>27</v>
@@ -16524,7 +16524,7 @@
       </c>
       <c r="B187" s="12"/>
       <c r="C187" s="29" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D187" s="12" t="s">
         <v>27</v>
@@ -16609,7 +16609,7 @@
       </c>
       <c r="B191" s="12"/>
       <c r="C191" s="134" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="D191" s="139" t="s">
         <v>27</v>
@@ -16694,7 +16694,7 @@
       </c>
       <c r="B195" s="12"/>
       <c r="C195" s="29" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="D195" s="12" t="s">
         <v>27</v>
@@ -16780,7 +16780,7 @@
       </c>
       <c r="B199" s="12"/>
       <c r="C199" s="134" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D199" s="12" t="s">
         <v>27</v>
@@ -16866,7 +16866,7 @@
       </c>
       <c r="B203" s="12"/>
       <c r="C203" s="134" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="D203" s="139" t="s">
         <v>27</v>
@@ -16929,7 +16929,7 @@
       </c>
       <c r="B206" s="120"/>
       <c r="C206" s="122" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D206" s="123" t="s">
         <v>8</v>
@@ -17003,7 +17003,7 @@
       </c>
       <c r="B209" s="12"/>
       <c r="C209" s="26" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D209" s="7" t="s">
         <v>143</v>
@@ -17026,7 +17026,7 @@
       </c>
       <c r="B210" s="12"/>
       <c r="C210" s="26" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D210" s="7" t="s">
         <v>143</v>
@@ -17491,7 +17491,7 @@
     <row r="223" spans="1:28" ht="20.100000000000001" customHeight="1">
       <c r="B223" s="197"/>
       <c r="C223" s="204" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D223" s="228" t="s">
         <v>8</v>
@@ -17514,7 +17514,7 @@
     </row>
     <row r="224" spans="1:28" s="9" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A224" s="252" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B224" s="12"/>
       <c r="C224" s="26" t="s">
@@ -17537,7 +17537,7 @@
     </row>
     <row r="225" spans="1:28" s="9" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A225" s="252" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B225" s="12"/>
       <c r="C225" s="26" t="s">
@@ -17560,7 +17560,7 @@
     </row>
     <row r="226" spans="1:28" s="9" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A226" s="252" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B226" s="12"/>
       <c r="C226" s="26" t="s">
@@ -17803,7 +17803,7 @@
     <row r="239" spans="1:28" s="86" customFormat="1" ht="35.1" customHeight="1">
       <c r="B239" s="88"/>
       <c r="C239" s="124" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="D239" s="125" t="s">
         <v>8</v>
@@ -17840,7 +17840,7 @@
     </row>
     <row r="240" spans="1:28" s="87" customFormat="1" outlineLevel="1">
       <c r="A240" s="87" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="B240" s="12"/>
       <c r="C240" s="26" t="s">
@@ -17863,7 +17863,7 @@
     </row>
     <row r="241" spans="1:13" s="87" customFormat="1" outlineLevel="1">
       <c r="A241" s="87" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="B241" s="12"/>
       <c r="C241" s="150" t="s">
@@ -17886,7 +17886,7 @@
     </row>
     <row r="242" spans="1:13" s="87" customFormat="1" outlineLevel="1">
       <c r="A242" s="87" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="B242" s="12"/>
       <c r="C242" s="150" t="s">
@@ -17909,11 +17909,11 @@
     </row>
     <row r="243" spans="1:13" s="87" customFormat="1" outlineLevel="1">
       <c r="A243" s="253" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B243" s="12"/>
       <c r="C243" s="26" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D243" s="86" t="s">
         <v>33</v>
@@ -17932,11 +17932,11 @@
     </row>
     <row r="244" spans="1:13" s="87" customFormat="1" outlineLevel="1">
       <c r="A244" s="253" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B244" s="12"/>
       <c r="C244" s="26" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D244" s="86" t="s">
         <v>33</v>
@@ -17955,14 +17955,14 @@
     </row>
     <row r="245" spans="1:13" s="87" customFormat="1" outlineLevel="1">
       <c r="A245" s="253" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B245" s="12"/>
       <c r="C245" s="26" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D245" s="86" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="E245" s="111" t="s">
         <v>100</v>
@@ -18211,7 +18211,7 @@
         <v>168</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>169</v>
@@ -18237,17 +18237,17 @@
       <c r="L3" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="M3" s="270" t="s">
+      <c r="M3" s="256" t="s">
         <v>372</v>
       </c>
-      <c r="N3" s="270" t="s">
-        <v>953</v>
-      </c>
-      <c r="O3" s="270" t="s">
+      <c r="N3" s="256" t="s">
+        <v>951</v>
+      </c>
+      <c r="O3" s="256" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="27" thickBot="1">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>126</v>
       </c>
@@ -18284,13 +18284,13 @@
       <c r="L4" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="M4" s="270" t="s">
+      <c r="M4" s="256" t="s">
         <v>373</v>
       </c>
-      <c r="N4" s="270" t="s">
+      <c r="N4" s="256" t="s">
         <v>491</v>
       </c>
-      <c r="O4" s="270" t="s">
+      <c r="O4" s="256" t="s">
         <v>576</v>
       </c>
     </row>
@@ -18302,7 +18302,7 @@
         <v>122</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>181</v>
@@ -18331,13 +18331,13 @@
       <c r="L5" s="2" t="s">
         <v>367</v>
       </c>
-      <c r="M5" s="270" t="s">
+      <c r="M5" s="256" t="s">
         <v>374</v>
       </c>
-      <c r="N5" s="270" t="s">
-        <v>943</v>
-      </c>
-      <c r="O5" s="270" t="s">
+      <c r="N5" s="256" t="s">
+        <v>941</v>
+      </c>
+      <c r="O5" s="256" t="s">
         <v>577</v>
       </c>
     </row>
@@ -18355,7 +18355,7 @@
         <v>188</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>189</v>
@@ -18372,13 +18372,13 @@
       <c r="K6" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="M6" s="270" t="s">
+      <c r="M6" s="256" t="s">
         <v>375</v>
       </c>
-      <c r="N6" s="270" t="s">
-        <v>944</v>
-      </c>
-      <c r="O6" s="270" t="s">
+      <c r="N6" s="256" t="s">
+        <v>942</v>
+      </c>
+      <c r="O6" s="256" t="s">
         <v>578</v>
       </c>
     </row>
@@ -18393,13 +18393,13 @@
         <v>192</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>193</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>194</v>
@@ -18410,13 +18410,13 @@
       <c r="K7" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="M7" s="270" t="s">
+      <c r="M7" s="256" t="s">
         <v>376</v>
       </c>
-      <c r="N7" s="270" t="s">
+      <c r="N7" s="256" t="s">
         <v>492</v>
       </c>
-      <c r="O7" s="270" t="s">
+      <c r="O7" s="256" t="s">
         <v>579</v>
       </c>
     </row>
@@ -18439,14 +18439,14 @@
       <c r="K8" s="2" t="s">
         <v>361</v>
       </c>
-      <c r="M8" s="270" t="s">
+      <c r="M8" s="256" t="s">
         <v>377</v>
       </c>
-      <c r="N8" s="270" t="s">
+      <c r="N8" s="256" t="s">
         <v>493</v>
       </c>
-      <c r="O8" s="270" t="s">
-        <v>958</v>
+      <c r="O8" s="256" t="s">
+        <v>956</v>
       </c>
     </row>
     <row r="9" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18465,13 +18465,13 @@
       <c r="K9" s="2" t="s">
         <v>362</v>
       </c>
-      <c r="M9" s="270" t="s">
-        <v>922</v>
-      </c>
-      <c r="N9" s="270" t="s">
+      <c r="M9" s="256" t="s">
+        <v>920</v>
+      </c>
+      <c r="N9" s="256" t="s">
         <v>494</v>
       </c>
-      <c r="O9" s="270" t="s">
+      <c r="O9" s="256" t="s">
         <v>580</v>
       </c>
     </row>
@@ -18491,13 +18491,13 @@
       <c r="K10" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="M10" s="270" t="s">
+      <c r="M10" s="256" t="s">
         <v>378</v>
       </c>
-      <c r="N10" s="270" t="s">
+      <c r="N10" s="256" t="s">
         <v>495</v>
       </c>
-      <c r="O10" s="270" t="s">
+      <c r="O10" s="256" t="s">
         <v>581</v>
       </c>
     </row>
@@ -18517,19 +18517,19 @@
       <c r="K11" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="M11" s="270" t="s">
+      <c r="M11" s="256" t="s">
         <v>379</v>
       </c>
-      <c r="N11" s="270" t="s">
+      <c r="N11" s="256" t="s">
         <v>496</v>
       </c>
-      <c r="O11" s="270" t="s">
+      <c r="O11" s="256" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="12" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="D12" s="1" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>208</v>
@@ -18540,13 +18540,13 @@
       <c r="J12" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="M12" s="270" t="s">
-        <v>923</v>
-      </c>
-      <c r="N12" s="270" t="s">
+      <c r="M12" s="256" t="s">
+        <v>921</v>
+      </c>
+      <c r="N12" s="256" t="s">
         <v>497</v>
       </c>
-      <c r="O12" s="270" t="s">
+      <c r="O12" s="256" t="s">
         <v>583</v>
       </c>
     </row>
@@ -18560,19 +18560,19 @@
       <c r="J13" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="M13" s="270" t="s">
+      <c r="M13" s="256" t="s">
         <v>380</v>
       </c>
-      <c r="N13" s="270" t="s">
+      <c r="N13" s="256" t="s">
         <v>498</v>
       </c>
-      <c r="O13" s="270" t="s">
+      <c r="O13" s="256" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="G14" s="9" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>233</v>
@@ -18580,13 +18580,13 @@
       <c r="J14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="M14" s="270" t="s">
+      <c r="M14" s="256" t="s">
         <v>381</v>
       </c>
-      <c r="N14" s="270" t="s">
+      <c r="N14" s="256" t="s">
         <v>499</v>
       </c>
-      <c r="O14" s="270" t="s">
+      <c r="O14" s="256" t="s">
         <v>585</v>
       </c>
     </row>
@@ -18597,14 +18597,14 @@
       <c r="J15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="M15" s="270" t="s">
+      <c r="M15" s="256" t="s">
         <v>382</v>
       </c>
-      <c r="N15" s="270" t="s">
-        <v>945</v>
-      </c>
-      <c r="O15" s="270" t="s">
-        <v>957</v>
+      <c r="N15" s="256" t="s">
+        <v>943</v>
+      </c>
+      <c r="O15" s="256" t="s">
+        <v>955</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18614,13 +18614,13 @@
       <c r="J16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M16" s="270" t="s">
-        <v>926</v>
-      </c>
-      <c r="N16" s="270" t="s">
+      <c r="M16" s="256" t="s">
+        <v>924</v>
+      </c>
+      <c r="N16" s="256" t="s">
         <v>500</v>
       </c>
-      <c r="O16" s="270" t="s">
+      <c r="O16" s="256" t="s">
         <v>651</v>
       </c>
     </row>
@@ -18631,13 +18631,13 @@
       <c r="J17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M17" s="270" t="s">
+      <c r="M17" s="256" t="s">
         <v>384</v>
       </c>
-      <c r="N17" s="270" t="s">
+      <c r="N17" s="256" t="s">
         <v>501</v>
       </c>
-      <c r="O17" s="270" t="s">
+      <c r="O17" s="256" t="s">
         <v>586</v>
       </c>
     </row>
@@ -18648,13 +18648,13 @@
       <c r="J18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="M18" s="270" t="s">
+      <c r="M18" s="256" t="s">
         <v>383</v>
       </c>
-      <c r="N18" s="270" t="s">
+      <c r="N18" s="256" t="s">
         <v>502</v>
       </c>
-      <c r="O18" s="270" t="s">
+      <c r="O18" s="256" t="s">
         <v>587</v>
       </c>
     </row>
@@ -18665,13 +18665,13 @@
       <c r="J19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="M19" s="270" t="s">
-        <v>925</v>
-      </c>
-      <c r="N19" s="270" t="s">
+      <c r="M19" s="256" t="s">
+        <v>923</v>
+      </c>
+      <c r="N19" s="256" t="s">
         <v>503</v>
       </c>
-      <c r="O19" s="270" t="s">
+      <c r="O19" s="256" t="s">
         <v>588</v>
       </c>
     </row>
@@ -18682,13 +18682,13 @@
       <c r="J20" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M20" s="270" t="s">
+      <c r="M20" s="256" t="s">
         <v>385</v>
       </c>
-      <c r="N20" s="270" t="s">
+      <c r="N20" s="256" t="s">
         <v>504</v>
       </c>
-      <c r="O20" s="270" t="s">
+      <c r="O20" s="256" t="s">
         <v>589</v>
       </c>
     </row>
@@ -18699,13 +18699,13 @@
       <c r="J21" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="M21" s="270" t="s">
+      <c r="M21" s="256" t="s">
         <v>386</v>
       </c>
-      <c r="N21" s="270" t="s">
+      <c r="N21" s="256" t="s">
         <v>538</v>
       </c>
-      <c r="O21" s="270" t="s">
+      <c r="O21" s="256" t="s">
         <v>590</v>
       </c>
     </row>
@@ -18716,13 +18716,13 @@
       <c r="J22" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M22" s="270" t="s">
+      <c r="M22" s="256" t="s">
         <v>387</v>
       </c>
-      <c r="N22" s="270" t="s">
+      <c r="N22" s="256" t="s">
         <v>505</v>
       </c>
-      <c r="O22" s="270" t="s">
+      <c r="O22" s="256" t="s">
         <v>591</v>
       </c>
     </row>
@@ -18733,13 +18733,13 @@
       <c r="J23" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="M23" s="270" t="s">
+      <c r="M23" s="256" t="s">
         <v>388</v>
       </c>
-      <c r="N23" s="270" t="s">
+      <c r="N23" s="256" t="s">
         <v>506</v>
       </c>
-      <c r="O23" s="270" t="s">
+      <c r="O23" s="256" t="s">
         <v>652</v>
       </c>
     </row>
@@ -18750,14 +18750,14 @@
       <c r="J24" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="M24" s="270" t="s">
+      <c r="M24" s="256" t="s">
         <v>389</v>
       </c>
-      <c r="N24" s="270" t="s">
-        <v>946</v>
-      </c>
-      <c r="O24" s="270" t="s">
-        <v>959</v>
+      <c r="N24" s="256" t="s">
+        <v>944</v>
+      </c>
+      <c r="O24" s="256" t="s">
+        <v>957</v>
       </c>
     </row>
     <row r="25" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18767,13 +18767,13 @@
       <c r="J25" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="M25" s="270" t="s">
+      <c r="M25" s="256" t="s">
         <v>390</v>
       </c>
-      <c r="N25" s="270" t="s">
+      <c r="N25" s="256" t="s">
         <v>507</v>
       </c>
-      <c r="O25" s="270" t="s">
+      <c r="O25" s="256" t="s">
         <v>592</v>
       </c>
     </row>
@@ -18784,13 +18784,13 @@
       <c r="J26" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="M26" s="270" t="s">
+      <c r="M26" s="256" t="s">
         <v>391</v>
       </c>
-      <c r="N26" s="270" t="s">
+      <c r="N26" s="256" t="s">
         <v>508</v>
       </c>
-      <c r="O26" s="270" t="s">
+      <c r="O26" s="256" t="s">
         <v>593</v>
       </c>
     </row>
@@ -18801,13 +18801,13 @@
       <c r="J27" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="M27" s="270" t="s">
+      <c r="M27" s="256" t="s">
         <v>392</v>
       </c>
-      <c r="N27" s="270" t="s">
+      <c r="N27" s="256" t="s">
         <v>509</v>
       </c>
-      <c r="O27" s="270" t="s">
+      <c r="O27" s="256" t="s">
         <v>594</v>
       </c>
     </row>
@@ -18818,13 +18818,13 @@
       <c r="J28" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="M28" s="270" t="s">
+      <c r="M28" s="256" t="s">
         <v>393</v>
       </c>
-      <c r="N28" s="270" t="s">
+      <c r="N28" s="256" t="s">
         <v>510</v>
       </c>
-      <c r="O28" s="270" t="s">
+      <c r="O28" s="256" t="s">
         <v>594</v>
       </c>
     </row>
@@ -18835,13 +18835,13 @@
       <c r="J29" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M29" s="270" t="s">
+      <c r="M29" s="256" t="s">
         <v>394</v>
       </c>
-      <c r="N29" s="270" t="s">
-        <v>947</v>
-      </c>
-      <c r="O29" s="270" t="s">
+      <c r="N29" s="256" t="s">
+        <v>945</v>
+      </c>
+      <c r="O29" s="256" t="s">
         <v>595</v>
       </c>
     </row>
@@ -18852,13 +18852,13 @@
       <c r="J30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M30" s="270" t="s">
-        <v>927</v>
-      </c>
-      <c r="N30" s="270" t="s">
+      <c r="M30" s="256" t="s">
+        <v>925</v>
+      </c>
+      <c r="N30" s="256" t="s">
         <v>511</v>
       </c>
-      <c r="O30" s="270" t="s">
+      <c r="O30" s="256" t="s">
         <v>596</v>
       </c>
     </row>
@@ -18869,13 +18869,13 @@
       <c r="J31" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="M31" s="270" t="s">
+      <c r="M31" s="256" t="s">
         <v>395</v>
       </c>
-      <c r="N31" s="270" t="s">
+      <c r="N31" s="256" t="s">
         <v>512</v>
       </c>
-      <c r="O31" s="270" t="s">
+      <c r="O31" s="256" t="s">
         <v>653</v>
       </c>
     </row>
@@ -18886,13 +18886,13 @@
       <c r="J32" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="M32" s="270" t="s">
+      <c r="M32" s="256" t="s">
         <v>396</v>
       </c>
-      <c r="N32" s="270" t="s">
-        <v>948</v>
-      </c>
-      <c r="O32" s="270" t="s">
+      <c r="N32" s="256" t="s">
+        <v>946</v>
+      </c>
+      <c r="O32" s="256" t="s">
         <v>597</v>
       </c>
     </row>
@@ -18903,14 +18903,14 @@
       <c r="J33" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="M33" s="270" t="s">
+      <c r="M33" s="256" t="s">
         <v>397</v>
       </c>
-      <c r="N33" s="270" t="s">
+      <c r="N33" s="256" t="s">
         <v>513</v>
       </c>
-      <c r="O33" s="270" t="s">
-        <v>960</v>
+      <c r="O33" s="256" t="s">
+        <v>958</v>
       </c>
     </row>
     <row r="34" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18920,13 +18920,13 @@
       <c r="J34" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M34" s="270" t="s">
+      <c r="M34" s="256" t="s">
         <v>398</v>
       </c>
-      <c r="N34" s="270" t="s">
+      <c r="N34" s="256" t="s">
         <v>514</v>
       </c>
-      <c r="O34" s="270" t="s">
+      <c r="O34" s="256" t="s">
         <v>654</v>
       </c>
     </row>
@@ -18937,13 +18937,13 @@
       <c r="J35" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="M35" s="270" t="s">
+      <c r="M35" s="256" t="s">
         <v>399</v>
       </c>
-      <c r="N35" s="270" t="s">
+      <c r="N35" s="256" t="s">
         <v>515</v>
       </c>
-      <c r="O35" s="270" t="s">
+      <c r="O35" s="256" t="s">
         <v>598</v>
       </c>
     </row>
@@ -18954,13 +18954,13 @@
       <c r="J36" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="M36" s="270" t="s">
+      <c r="M36" s="256" t="s">
         <v>400</v>
       </c>
-      <c r="N36" s="270" t="s">
+      <c r="N36" s="256" t="s">
         <v>516</v>
       </c>
-      <c r="O36" s="270" t="s">
+      <c r="O36" s="256" t="s">
         <v>599</v>
       </c>
     </row>
@@ -18968,27 +18968,27 @@
       <c r="J37" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="M37" s="270" t="s">
-        <v>928</v>
-      </c>
-      <c r="N37" s="270" t="s">
-        <v>949</v>
-      </c>
-      <c r="O37" s="270" t="s">
-        <v>961</v>
+      <c r="M37" s="256" t="s">
+        <v>926</v>
+      </c>
+      <c r="N37" s="256" t="s">
+        <v>947</v>
+      </c>
+      <c r="O37" s="256" t="s">
+        <v>959</v>
       </c>
     </row>
     <row r="38" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="J38" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="M38" s="270" t="s">
+      <c r="M38" s="256" t="s">
         <v>401</v>
       </c>
-      <c r="N38" s="270" t="s">
+      <c r="N38" s="256" t="s">
         <v>517</v>
       </c>
-      <c r="O38" s="270" t="s">
+      <c r="O38" s="256" t="s">
         <v>600</v>
       </c>
     </row>
@@ -18996,919 +18996,919 @@
       <c r="J39" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="M39" s="270" t="s">
+      <c r="M39" s="256" t="s">
         <v>402</v>
       </c>
-      <c r="N39" s="270" t="s">
+      <c r="N39" s="256" t="s">
         <v>518</v>
       </c>
-      <c r="O39" s="270" t="s">
+      <c r="O39" s="256" t="s">
         <v>601</v>
       </c>
     </row>
     <row r="40" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M40" s="270" t="s">
+      <c r="M40" s="256" t="s">
         <v>403</v>
       </c>
-      <c r="N40" s="270" t="s">
+      <c r="N40" s="256" t="s">
         <v>519</v>
       </c>
-      <c r="O40" s="270" t="s">
+      <c r="O40" s="256" t="s">
         <v>602</v>
       </c>
     </row>
     <row r="41" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M41" s="270" t="s">
-        <v>924</v>
-      </c>
-      <c r="N41" s="270" t="s">
+      <c r="M41" s="256" t="s">
+        <v>922</v>
+      </c>
+      <c r="N41" s="256" t="s">
         <v>520</v>
       </c>
-      <c r="O41" s="270" t="s">
+      <c r="O41" s="256" t="s">
         <v>603</v>
       </c>
     </row>
     <row r="42" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M42" s="270" t="s">
+      <c r="M42" s="256" t="s">
         <v>405</v>
       </c>
-      <c r="N42" s="270" t="s">
+      <c r="N42" s="256" t="s">
         <v>521</v>
       </c>
-      <c r="O42" s="270" t="s">
+      <c r="O42" s="256" t="s">
         <v>604</v>
       </c>
     </row>
     <row r="43" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M43" s="270" t="s">
+      <c r="M43" s="256" t="s">
         <v>406</v>
       </c>
-      <c r="N43" s="270" t="s">
+      <c r="N43" s="256" t="s">
         <v>522</v>
       </c>
-      <c r="O43" s="270" t="s">
+      <c r="O43" s="256" t="s">
         <v>605</v>
       </c>
     </row>
     <row r="44" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
-      <c r="M44" s="270" t="s">
+      <c r="M44" s="256" t="s">
         <v>407</v>
       </c>
-      <c r="N44" s="270" t="s">
+      <c r="N44" s="256" t="s">
         <v>523</v>
       </c>
-      <c r="O44" s="270" t="s">
+      <c r="O44" s="256" t="s">
         <v>606</v>
       </c>
     </row>
     <row r="45" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M45" s="270" t="s">
+      <c r="M45" s="256" t="s">
         <v>408</v>
       </c>
-      <c r="N45" s="270" t="s">
+      <c r="N45" s="256" t="s">
         <v>524</v>
       </c>
-      <c r="O45" s="270" t="s">
+      <c r="O45" s="256" t="s">
         <v>607</v>
       </c>
     </row>
     <row r="46" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M46" s="270" t="s">
+      <c r="M46" s="256" t="s">
         <v>409</v>
       </c>
-      <c r="N46" s="270" t="s">
+      <c r="N46" s="256" t="s">
         <v>525</v>
       </c>
-      <c r="O46" s="270" t="s">
+      <c r="O46" s="256" t="s">
         <v>608</v>
       </c>
     </row>
     <row r="47" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M47" s="270" t="s">
+      <c r="M47" s="256" t="s">
         <v>410</v>
       </c>
-      <c r="N47" s="270" t="s">
+      <c r="N47" s="256" t="s">
         <v>526</v>
       </c>
-      <c r="O47" s="270" t="s">
+      <c r="O47" s="256" t="s">
         <v>609</v>
       </c>
     </row>
     <row r="48" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M48" s="270" t="s">
+      <c r="M48" s="256" t="s">
         <v>411</v>
       </c>
-      <c r="N48" s="270" t="s">
+      <c r="N48" s="256" t="s">
         <v>527</v>
       </c>
-      <c r="O48" s="270" t="s">
+      <c r="O48" s="256" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="49" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M49" s="256" t="s">
+        <v>412</v>
+      </c>
+      <c r="N49" s="256" t="s">
+        <v>528</v>
+      </c>
+      <c r="O49" s="256" t="s">
+        <v>961</v>
+      </c>
+    </row>
+    <row r="50" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M50" s="256" t="s">
+        <v>404</v>
+      </c>
+      <c r="N50" s="256" t="s">
+        <v>529</v>
+      </c>
+      <c r="O50" s="256" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="51" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M51" s="256" t="s">
+        <v>413</v>
+      </c>
+      <c r="N51" s="256" t="s">
+        <v>530</v>
+      </c>
+      <c r="O51" s="256" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="52" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M52" s="256" t="s">
+        <v>414</v>
+      </c>
+      <c r="N52" s="256" t="s">
+        <v>940</v>
+      </c>
+      <c r="O52" s="256" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="53" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="M53" s="256" t="s">
+        <v>415</v>
+      </c>
+      <c r="N53" s="256" t="s">
+        <v>574</v>
+      </c>
+      <c r="O53" s="256" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="54" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M54" s="256" t="s">
+        <v>416</v>
+      </c>
+      <c r="N54" s="256" t="s">
+        <v>531</v>
+      </c>
+      <c r="O54" s="256" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="55" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="M55" s="256" t="s">
+        <v>927</v>
+      </c>
+      <c r="N55" s="256" t="s">
+        <v>532</v>
+      </c>
+      <c r="O55" s="256" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="56" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="M56" s="256" t="s">
+        <v>928</v>
+      </c>
+      <c r="N56" s="256" t="s">
+        <v>948</v>
+      </c>
+      <c r="O56" s="256" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="57" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M57" s="256" t="s">
+        <v>417</v>
+      </c>
+      <c r="N57" s="256" t="s">
+        <v>533</v>
+      </c>
+      <c r="O57" s="256" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="58" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M58" s="256" t="s">
+        <v>418</v>
+      </c>
+      <c r="N58" s="256" t="s">
+        <v>534</v>
+      </c>
+      <c r="O58" s="256" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="59" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M59" s="256" t="s">
+        <v>419</v>
+      </c>
+      <c r="N59" s="256" t="s">
+        <v>535</v>
+      </c>
+      <c r="O59" s="256" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="60" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M60" s="256" t="s">
+        <v>420</v>
+      </c>
+      <c r="N60" s="256" t="s">
+        <v>536</v>
+      </c>
+      <c r="O60" s="256" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="61" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M61" s="256" t="s">
+        <v>421</v>
+      </c>
+      <c r="N61" s="256" t="s">
+        <v>537</v>
+      </c>
+      <c r="O61" s="256" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="62" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M62" s="256" t="s">
+        <v>422</v>
+      </c>
+      <c r="N62" s="256" t="s">
+        <v>539</v>
+      </c>
+      <c r="O62" s="256" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="63" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M63" s="256" t="s">
+        <v>929</v>
+      </c>
+      <c r="N63" s="256" t="s">
+        <v>540</v>
+      </c>
+      <c r="O63" s="256" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="64" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M64" s="256" t="s">
+        <v>423</v>
+      </c>
+      <c r="N64" s="256" t="s">
+        <v>541</v>
+      </c>
+      <c r="O64" s="256" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="65" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="M65" s="256" t="s">
+        <v>930</v>
+      </c>
+      <c r="N65" s="256" t="s">
+        <v>542</v>
+      </c>
+      <c r="O65" s="256" t="s">
         <v>962</v>
       </c>
     </row>
-    <row r="49" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M49" s="270" t="s">
-        <v>412</v>
-      </c>
-      <c r="N49" s="270" t="s">
-        <v>528</v>
-      </c>
-      <c r="O49" s="270" t="s">
+    <row r="66" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="M66" s="256" t="s">
+        <v>424</v>
+      </c>
+      <c r="N66" s="256" t="s">
+        <v>949</v>
+      </c>
+      <c r="O66" s="256" t="s">
         <v>963</v>
       </c>
     </row>
-    <row r="50" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M50" s="270" t="s">
-        <v>404</v>
-      </c>
-      <c r="N50" s="270" t="s">
-        <v>529</v>
-      </c>
-      <c r="O50" s="270" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="51" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M51" s="270" t="s">
-        <v>413</v>
-      </c>
-      <c r="N51" s="270" t="s">
-        <v>530</v>
-      </c>
-      <c r="O51" s="270" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="52" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M52" s="270" t="s">
-        <v>414</v>
-      </c>
-      <c r="N52" s="270" t="s">
-        <v>942</v>
-      </c>
-      <c r="O52" s="270" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="53" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
-      <c r="M53" s="270" t="s">
-        <v>415</v>
-      </c>
-      <c r="N53" s="270" t="s">
+    <row r="67" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M67" s="256" t="s">
+        <v>425</v>
+      </c>
+      <c r="N67" s="256" t="s">
+        <v>950</v>
+      </c>
+      <c r="O67" s="256" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="68" spans="13:15" ht="27" thickBot="1">
+      <c r="M68" s="256" t="s">
+        <v>426</v>
+      </c>
+      <c r="N68" s="256" t="s">
+        <v>543</v>
+      </c>
+      <c r="O68" s="256" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="69" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M69" s="256" t="s">
+        <v>932</v>
+      </c>
+      <c r="N69" s="256" t="s">
+        <v>544</v>
+      </c>
+      <c r="O69" s="256" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="70" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M70" s="256" t="s">
+        <v>933</v>
+      </c>
+      <c r="N70" s="256" t="s">
+        <v>545</v>
+      </c>
+      <c r="O70" s="256" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="71" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M71" s="256" t="s">
+        <v>427</v>
+      </c>
+      <c r="N71" s="256" t="s">
+        <v>916</v>
+      </c>
+      <c r="O71" s="256" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="72" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M72" s="256" t="s">
+        <v>428</v>
+      </c>
+      <c r="N72" s="256" t="s">
+        <v>546</v>
+      </c>
+      <c r="O72" s="256" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="73" spans="13:15" ht="27" thickBot="1">
+      <c r="M73" s="256" t="s">
+        <v>429</v>
+      </c>
+      <c r="N73" s="256" t="s">
+        <v>547</v>
+      </c>
+      <c r="O73" s="256" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="74" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M74" s="256" t="s">
+        <v>430</v>
+      </c>
+      <c r="N74" s="256" t="s">
+        <v>548</v>
+      </c>
+      <c r="O74" s="256" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="75" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M75" s="256" t="s">
+        <v>934</v>
+      </c>
+      <c r="N75" s="256" t="s">
+        <v>549</v>
+      </c>
+      <c r="O75" s="256" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="76" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M76" s="256" t="s">
+        <v>432</v>
+      </c>
+      <c r="N76" s="256" t="s">
+        <v>550</v>
+      </c>
+      <c r="O76" s="256" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="77" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M77" s="256" t="s">
+        <v>431</v>
+      </c>
+      <c r="N77" s="256" t="s">
+        <v>551</v>
+      </c>
+      <c r="O77" s="256" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="78" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M78" s="256" t="s">
+        <v>433</v>
+      </c>
+      <c r="N78" s="256" t="s">
+        <v>552</v>
+      </c>
+      <c r="O78" s="256" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="79" spans="13:15" ht="27" thickBot="1">
+      <c r="M79" s="256" t="s">
+        <v>434</v>
+      </c>
+      <c r="N79" s="256" t="s">
+        <v>553</v>
+      </c>
+      <c r="O79" s="256" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="80" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M80" s="256" t="s">
+        <v>435</v>
+      </c>
+      <c r="N80" s="256" t="s">
+        <v>952</v>
+      </c>
+      <c r="O80" s="256" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="81" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M81" s="256" t="s">
+        <v>436</v>
+      </c>
+      <c r="N81" s="256" t="s">
+        <v>554</v>
+      </c>
+      <c r="O81" s="256" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="82" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M82" s="256" t="s">
+        <v>437</v>
+      </c>
+      <c r="N82" s="256" t="s">
+        <v>555</v>
+      </c>
+      <c r="O82" s="256" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="83" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M83" s="256" t="s">
+        <v>438</v>
+      </c>
+      <c r="N83" s="256" t="s">
+        <v>953</v>
+      </c>
+      <c r="O83" s="256" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="84" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M84" s="256" t="s">
+        <v>439</v>
+      </c>
+      <c r="N84" s="256" t="s">
+        <v>556</v>
+      </c>
+      <c r="O84" s="256" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="85" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M85" s="256" t="s">
+        <v>440</v>
+      </c>
+      <c r="N85" s="256" t="s">
+        <v>557</v>
+      </c>
+      <c r="O85" s="256" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="86" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M86" s="256" t="s">
+        <v>441</v>
+      </c>
+      <c r="N86" s="256" t="s">
+        <v>558</v>
+      </c>
+      <c r="O86" s="256" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="87" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M87" s="256" t="s">
+        <v>442</v>
+      </c>
+      <c r="N87" s="256" t="s">
+        <v>559</v>
+      </c>
+      <c r="O87" s="256" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="88" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M88" s="256" t="s">
+        <v>443</v>
+      </c>
+      <c r="N88" s="256" t="s">
+        <v>560</v>
+      </c>
+      <c r="O88" s="256" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="89" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M89" s="256" t="s">
+        <v>444</v>
+      </c>
+      <c r="N89" s="256" t="s">
+        <v>561</v>
+      </c>
+      <c r="O89" s="256" t="s">
+        <v>970</v>
+      </c>
+    </row>
+    <row r="90" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M90" s="256" t="s">
+        <v>445</v>
+      </c>
+      <c r="N90" s="256" t="s">
+        <v>954</v>
+      </c>
+      <c r="O90" s="256" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="91" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M91" s="256" t="s">
+        <v>446</v>
+      </c>
+      <c r="N91" s="256" t="s">
+        <v>562</v>
+      </c>
+      <c r="O91" s="256" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="92" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M92" s="256" t="s">
+        <v>447</v>
+      </c>
+      <c r="N92" s="256" t="s">
+        <v>563</v>
+      </c>
+      <c r="O92" s="256" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="93" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M93" s="256" t="s">
+        <v>937</v>
+      </c>
+      <c r="N93" s="256" t="s">
+        <v>564</v>
+      </c>
+      <c r="O93" s="256" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="94" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M94" s="256" t="s">
+        <v>448</v>
+      </c>
+      <c r="N94" s="256" t="s">
+        <v>565</v>
+      </c>
+      <c r="O94" s="256" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="95" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M95" s="256" t="s">
+        <v>449</v>
+      </c>
+      <c r="N95" s="256" t="s">
+        <v>566</v>
+      </c>
+      <c r="O95" s="256" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="96" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M96" s="256" t="s">
+        <v>450</v>
+      </c>
+      <c r="N96" s="256" t="s">
+        <v>567</v>
+      </c>
+      <c r="O96" s="256" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="97" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M97" s="256" t="s">
+        <v>451</v>
+      </c>
+      <c r="N97" s="256" t="s">
+        <v>568</v>
+      </c>
+      <c r="O97" s="256" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="98" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M98" s="256" t="s">
+        <v>452</v>
+      </c>
+      <c r="N98" s="256" t="s">
+        <v>569</v>
+      </c>
+      <c r="O98" s="256" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="99" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M99" s="256" t="s">
+        <v>453</v>
+      </c>
+      <c r="N99" s="256" t="s">
+        <v>570</v>
+      </c>
+      <c r="O99" s="256" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="100" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M100" s="256" t="s">
+        <v>454</v>
+      </c>
+      <c r="N100" s="256" t="s">
+        <v>571</v>
+      </c>
+      <c r="O100" s="256" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="101" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M101" s="256" t="s">
+        <v>455</v>
+      </c>
+      <c r="N101" s="256" t="s">
+        <v>572</v>
+      </c>
+      <c r="O101" s="256" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="102" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M102" s="256" t="s">
+        <v>456</v>
+      </c>
+      <c r="N102" s="256" t="s">
+        <v>573</v>
+      </c>
+      <c r="O102" s="256" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="103" spans="13:15" ht="27" thickBot="1">
+      <c r="M103" s="256" t="s">
+        <v>458</v>
+      </c>
+      <c r="N103" s="256" t="s">
         <v>574</v>
       </c>
-      <c r="O53" s="270" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="54" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M54" s="270" t="s">
-        <v>416</v>
-      </c>
-      <c r="N54" s="270" t="s">
-        <v>531</v>
-      </c>
-      <c r="O54" s="270" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="55" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
-      <c r="M55" s="270" t="s">
-        <v>929</v>
-      </c>
-      <c r="N55" s="270" t="s">
-        <v>532</v>
-      </c>
-      <c r="O55" s="270" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="56" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
-      <c r="M56" s="270" t="s">
-        <v>930</v>
-      </c>
-      <c r="N56" s="270" t="s">
-        <v>950</v>
-      </c>
-      <c r="O56" s="270" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="57" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M57" s="270" t="s">
-        <v>417</v>
-      </c>
-      <c r="N57" s="270" t="s">
-        <v>533</v>
-      </c>
-      <c r="O57" s="270" t="s">
-        <v>617</v>
-      </c>
-    </row>
-    <row r="58" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M58" s="270" t="s">
-        <v>418</v>
-      </c>
-      <c r="N58" s="270" t="s">
-        <v>534</v>
-      </c>
-      <c r="O58" s="270" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="59" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M59" s="270" t="s">
-        <v>419</v>
-      </c>
-      <c r="N59" s="270" t="s">
-        <v>535</v>
-      </c>
-      <c r="O59" s="270" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="60" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M60" s="270" t="s">
-        <v>420</v>
-      </c>
-      <c r="N60" s="270" t="s">
-        <v>536</v>
-      </c>
-      <c r="O60" s="270" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="61" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M61" s="270" t="s">
-        <v>421</v>
-      </c>
-      <c r="N61" s="270" t="s">
-        <v>537</v>
-      </c>
-      <c r="O61" s="270" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="62" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M62" s="270" t="s">
-        <v>422</v>
-      </c>
-      <c r="N62" s="270" t="s">
-        <v>539</v>
-      </c>
-      <c r="O62" s="270" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="63" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
-      <c r="M63" s="270" t="s">
+      <c r="O103" s="256" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="104" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M104" s="256" t="s">
+        <v>457</v>
+      </c>
+      <c r="O104" s="256" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="105" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M105" s="256" t="s">
+        <v>459</v>
+      </c>
+      <c r="O105" s="256" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="106" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M106" s="256" t="s">
+        <v>460</v>
+      </c>
+      <c r="O106" s="256" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="107" spans="13:15" ht="27" thickBot="1">
+      <c r="M107" s="256" t="s">
+        <v>461</v>
+      </c>
+      <c r="O107" s="256" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="108" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M108" s="256" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="109" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M109" s="256" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="110" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M110" s="256" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="111" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M111" s="256" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="112" spans="13:15" ht="15.75" thickBot="1">
+      <c r="M112" s="256" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="113" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M113" s="256" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="114" spans="13:13" ht="27" thickBot="1">
+      <c r="M114" s="256" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="115" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M115" s="256" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="116" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M116" s="256" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="117" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M117" s="256" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="118" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M118" s="256" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="119" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M119" s="256" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="120" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M120" s="256" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="121" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M121" s="256" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="122" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M122" s="256" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="123" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M123" s="256" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="124" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M124" s="256" t="s">
         <v>931</v>
       </c>
-      <c r="N63" s="270" t="s">
-        <v>540</v>
-      </c>
-      <c r="O63" s="270" t="s">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="64" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M64" s="270" t="s">
-        <v>423</v>
-      </c>
-      <c r="N64" s="270" t="s">
-        <v>541</v>
-      </c>
-      <c r="O64" s="270" t="s">
-        <v>623</v>
-      </c>
-    </row>
-    <row r="65" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
-      <c r="M65" s="270" t="s">
-        <v>932</v>
-      </c>
-      <c r="N65" s="270" t="s">
-        <v>542</v>
-      </c>
-      <c r="O65" s="270" t="s">
-        <v>964</v>
-      </c>
-    </row>
-    <row r="66" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="M66" s="270" t="s">
-        <v>424</v>
-      </c>
-      <c r="N66" s="270" t="s">
-        <v>951</v>
-      </c>
-      <c r="O66" s="270" t="s">
-        <v>965</v>
-      </c>
-    </row>
-    <row r="67" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M67" s="270" t="s">
-        <v>425</v>
-      </c>
-      <c r="N67" s="270" t="s">
-        <v>952</v>
-      </c>
-      <c r="O67" s="270" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="68" spans="13:15" ht="27" thickBot="1">
-      <c r="M68" s="270" t="s">
-        <v>426</v>
-      </c>
-      <c r="N68" s="270" t="s">
-        <v>543</v>
-      </c>
-      <c r="O68" s="270" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="69" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M69" s="270" t="s">
-        <v>934</v>
-      </c>
-      <c r="N69" s="270" t="s">
-        <v>544</v>
-      </c>
-      <c r="O69" s="270" t="s">
-        <v>626</v>
-      </c>
-    </row>
-    <row r="70" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M70" s="270" t="s">
-        <v>935</v>
-      </c>
-      <c r="N70" s="270" t="s">
-        <v>545</v>
-      </c>
-      <c r="O70" s="270" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="71" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M71" s="270" t="s">
-        <v>427</v>
-      </c>
-      <c r="N71" s="270" t="s">
-        <v>918</v>
-      </c>
-      <c r="O71" s="270" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="72" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M72" s="270" t="s">
-        <v>428</v>
-      </c>
-      <c r="N72" s="270" t="s">
-        <v>546</v>
-      </c>
-      <c r="O72" s="270" t="s">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="73" spans="13:15" ht="27" thickBot="1">
-      <c r="M73" s="270" t="s">
-        <v>429</v>
-      </c>
-      <c r="N73" s="270" t="s">
-        <v>547</v>
-      </c>
-      <c r="O73" s="270" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="74" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M74" s="270" t="s">
-        <v>430</v>
-      </c>
-      <c r="N74" s="270" t="s">
-        <v>548</v>
-      </c>
-      <c r="O74" s="270" t="s">
-        <v>968</v>
-      </c>
-    </row>
-    <row r="75" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M75" s="270" t="s">
-        <v>936</v>
-      </c>
-      <c r="N75" s="270" t="s">
-        <v>549</v>
-      </c>
-      <c r="O75" s="270" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="76" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M76" s="270" t="s">
-        <v>432</v>
-      </c>
-      <c r="N76" s="270" t="s">
-        <v>550</v>
-      </c>
-      <c r="O76" s="270" t="s">
-        <v>969</v>
-      </c>
-    </row>
-    <row r="77" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M77" s="270" t="s">
-        <v>431</v>
-      </c>
-      <c r="N77" s="270" t="s">
-        <v>551</v>
-      </c>
-      <c r="O77" s="270" t="s">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="78" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M78" s="270" t="s">
-        <v>433</v>
-      </c>
-      <c r="N78" s="270" t="s">
-        <v>552</v>
-      </c>
-      <c r="O78" s="270" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="79" spans="13:15" ht="27" thickBot="1">
-      <c r="M79" s="270" t="s">
-        <v>434</v>
-      </c>
-      <c r="N79" s="270" t="s">
-        <v>553</v>
-      </c>
-      <c r="O79" s="270" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="80" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M80" s="270" t="s">
-        <v>435</v>
-      </c>
-      <c r="N80" s="270" t="s">
-        <v>954</v>
-      </c>
-      <c r="O80" s="270" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="81" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M81" s="270" t="s">
-        <v>436</v>
-      </c>
-      <c r="N81" s="270" t="s">
-        <v>554</v>
-      </c>
-      <c r="O81" s="270" t="s">
-        <v>656</v>
-      </c>
-    </row>
-    <row r="82" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M82" s="270" t="s">
-        <v>437</v>
-      </c>
-      <c r="N82" s="270" t="s">
-        <v>555</v>
-      </c>
-      <c r="O82" s="270" t="s">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="83" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M83" s="270" t="s">
-        <v>438</v>
-      </c>
-      <c r="N83" s="270" t="s">
-        <v>955</v>
-      </c>
-      <c r="O83" s="270" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="84" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M84" s="270" t="s">
-        <v>439</v>
-      </c>
-      <c r="N84" s="270" t="s">
-        <v>556</v>
-      </c>
-      <c r="O84" s="270" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="85" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M85" s="270" t="s">
-        <v>440</v>
-      </c>
-      <c r="N85" s="270" t="s">
-        <v>557</v>
-      </c>
-      <c r="O85" s="270" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="86" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M86" s="270" t="s">
-        <v>441</v>
-      </c>
-      <c r="N86" s="270" t="s">
-        <v>558</v>
-      </c>
-      <c r="O86" s="270" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="87" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M87" s="270" t="s">
-        <v>442</v>
-      </c>
-      <c r="N87" s="270" t="s">
-        <v>559</v>
-      </c>
-      <c r="O87" s="270" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="88" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M88" s="270" t="s">
-        <v>443</v>
-      </c>
-      <c r="N88" s="270" t="s">
-        <v>560</v>
-      </c>
-      <c r="O88" s="270" t="s">
-        <v>973</v>
-      </c>
-    </row>
-    <row r="89" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M89" s="270" t="s">
-        <v>444</v>
-      </c>
-      <c r="N89" s="270" t="s">
-        <v>561</v>
-      </c>
-      <c r="O89" s="270" t="s">
-        <v>972</v>
-      </c>
-    </row>
-    <row r="90" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M90" s="270" t="s">
-        <v>445</v>
-      </c>
-      <c r="N90" s="270" t="s">
-        <v>956</v>
-      </c>
-      <c r="O90" s="270" t="s">
-        <v>967</v>
-      </c>
-    </row>
-    <row r="91" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M91" s="270" t="s">
-        <v>446</v>
-      </c>
-      <c r="N91" s="270" t="s">
-        <v>562</v>
-      </c>
-      <c r="O91" s="270" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="92" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M92" s="270" t="s">
-        <v>447</v>
-      </c>
-      <c r="N92" s="270" t="s">
-        <v>563</v>
-      </c>
-      <c r="O92" s="270" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="93" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M93" s="270" t="s">
+    </row>
+    <row r="125" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M125" s="256" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="126" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M126" s="256" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="127" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M127" s="256" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="128" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M128" s="256" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="129" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M129" s="256" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="130" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M130" s="256" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="131" spans="13:13" ht="15.75" thickBot="1">
+      <c r="M131" s="256" t="s">
         <v>939</v>
       </c>
-      <c r="N93" s="270" t="s">
-        <v>564</v>
-      </c>
-      <c r="O93" s="270" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="94" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M94" s="270" t="s">
-        <v>448</v>
-      </c>
-      <c r="N94" s="270" t="s">
-        <v>565</v>
-      </c>
-      <c r="O94" s="270" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="95" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M95" s="270" t="s">
-        <v>449</v>
-      </c>
-      <c r="N95" s="270" t="s">
-        <v>566</v>
-      </c>
-      <c r="O95" s="270" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="96" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M96" s="270" t="s">
-        <v>450</v>
-      </c>
-      <c r="N96" s="270" t="s">
-        <v>567</v>
-      </c>
-      <c r="O96" s="270" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="97" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M97" s="270" t="s">
-        <v>451</v>
-      </c>
-      <c r="N97" s="270" t="s">
-        <v>568</v>
-      </c>
-      <c r="O97" s="270" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="98" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M98" s="270" t="s">
-        <v>452</v>
-      </c>
-      <c r="N98" s="270" t="s">
-        <v>569</v>
-      </c>
-      <c r="O98" s="270" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="99" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M99" s="270" t="s">
-        <v>453</v>
-      </c>
-      <c r="N99" s="270" t="s">
-        <v>570</v>
-      </c>
-      <c r="O99" s="270" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="100" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M100" s="270" t="s">
-        <v>454</v>
-      </c>
-      <c r="N100" s="270" t="s">
-        <v>571</v>
-      </c>
-      <c r="O100" s="270" t="s">
-        <v>974</v>
-      </c>
-    </row>
-    <row r="101" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M101" s="270" t="s">
-        <v>455</v>
-      </c>
-      <c r="N101" s="270" t="s">
-        <v>572</v>
-      </c>
-      <c r="O101" s="270" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="102" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M102" s="270" t="s">
-        <v>456</v>
-      </c>
-      <c r="N102" s="270" t="s">
-        <v>573</v>
-      </c>
-      <c r="O102" s="270" t="s">
-        <v>975</v>
-      </c>
-    </row>
-    <row r="103" spans="13:15" ht="27" thickBot="1">
-      <c r="M103" s="270" t="s">
-        <v>458</v>
-      </c>
-      <c r="N103" s="270" t="s">
-        <v>574</v>
-      </c>
-      <c r="O103" s="270" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="104" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M104" s="270" t="s">
-        <v>457</v>
-      </c>
-      <c r="O104" s="270" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="105" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M105" s="270" t="s">
-        <v>459</v>
-      </c>
-      <c r="O105" s="270" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="106" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M106" s="270" t="s">
-        <v>460</v>
-      </c>
-      <c r="O106" s="270" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="107" spans="13:15" ht="27" thickBot="1">
-      <c r="M107" s="270" t="s">
-        <v>461</v>
-      </c>
-      <c r="O107" s="270" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="108" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M108" s="270" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="109" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M109" s="270" t="s">
-        <v>937</v>
-      </c>
-    </row>
-    <row r="110" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M110" s="270" t="s">
-        <v>938</v>
-      </c>
-    </row>
-    <row r="111" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M111" s="270" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="112" spans="13:15" ht="15.75" thickBot="1">
-      <c r="M112" s="270" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="113" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M113" s="270" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="114" spans="13:13" ht="27" thickBot="1">
-      <c r="M114" s="270" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="115" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M115" s="270" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="116" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M116" s="270" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="117" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M117" s="270" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="118" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M118" s="270" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="119" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M119" s="270" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="120" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M120" s="270" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="121" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M121" s="270" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="122" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M122" s="270" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="123" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M123" s="270" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="124" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M124" s="270" t="s">
-        <v>933</v>
-      </c>
-    </row>
-    <row r="125" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M125" s="270" t="s">
-        <v>476</v>
-      </c>
-    </row>
-    <row r="126" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M126" s="270" t="s">
-        <v>940</v>
-      </c>
-    </row>
-    <row r="127" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M127" s="270" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="128" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M128" s="270" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="129" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M129" s="270" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="130" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M130" s="270" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="131" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M131" s="270" t="s">
-        <v>941</v>
-      </c>
     </row>
     <row r="132" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M132" s="270" t="s">
+      <c r="M132" s="256" t="s">
         <v>481</v>
       </c>
     </row>
     <row r="133" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M133" s="270" t="s">
+      <c r="M133" s="256" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="134" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M134" s="270" t="s">
+      <c r="M134" s="256" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="135" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M135" s="270" t="s">
+      <c r="M135" s="256" t="s">
         <v>484</v>
       </c>
     </row>
     <row r="136" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M136" s="270" t="s">
+      <c r="M136" s="256" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="137" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M137" s="270" t="s">
+      <c r="M137" s="256" t="s">
         <v>486</v>
       </c>
     </row>
     <row r="138" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M138" s="270" t="s">
+      <c r="M138" s="256" t="s">
         <v>488</v>
       </c>
     </row>
     <row r="139" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M139" s="270" t="s">
+      <c r="M139" s="256" t="s">
         <v>487</v>
       </c>
     </row>
     <row r="140" spans="13:13" ht="15.75" thickBot="1">
-      <c r="M140" s="270" t="s">
+      <c r="M140" s="256" t="s">
         <v>489</v>
       </c>
     </row>
     <row r="141" spans="13:13" ht="27" thickBot="1">
-      <c r="M141" s="270" t="s">
+      <c r="M141" s="256" t="s">
         <v>490</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change transport and packaging model for ecoinvent, + add horticultural oil in these models + hide hidden column in template (oups)
</commit_message>
<xml_diff>
--- a/src/main/dart/web/LCI-Database_Data-collection_Crop_v1.xlsx
+++ b/src/main/dart/web/LCI-Database_Data-collection_Crop_v1.xlsx
@@ -5933,6 +5933,18 @@
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="49" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="51" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -5944,18 +5956,6 @@
     </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="49" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="51" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -8928,25 +8928,25 @@
     </row>
     <row r="5" spans="1:9" s="160" customFormat="1" ht="54.75" customHeight="1">
       <c r="A5" s="159"/>
-      <c r="B5" s="258"/>
-      <c r="C5" s="258"/>
-      <c r="D5" s="258"/>
-      <c r="E5" s="258"/>
-      <c r="F5" s="258"/>
-      <c r="G5" s="258"/>
+      <c r="B5" s="262"/>
+      <c r="C5" s="262"/>
+      <c r="D5" s="262"/>
+      <c r="E5" s="262"/>
+      <c r="F5" s="262"/>
+      <c r="G5" s="262"/>
       <c r="H5" s="156"/>
       <c r="I5" s="156"/>
     </row>
     <row r="6" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A6" s="154"/>
-      <c r="B6" s="259" t="s">
+      <c r="B6" s="263" t="s">
         <v>734</v>
       </c>
-      <c r="C6" s="259"/>
-      <c r="D6" s="259"/>
-      <c r="E6" s="259"/>
-      <c r="F6" s="259"/>
-      <c r="G6" s="259"/>
+      <c r="C6" s="263"/>
+      <c r="D6" s="263"/>
+      <c r="E6" s="263"/>
+      <c r="F6" s="263"/>
+      <c r="G6" s="263"/>
       <c r="H6" s="156"/>
       <c r="I6" s="156"/>
     </row>
@@ -8963,14 +8963,14 @@
     </row>
     <row r="8" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A8" s="154"/>
-      <c r="B8" s="260" t="s">
+      <c r="B8" s="264" t="s">
         <v>709</v>
       </c>
-      <c r="C8" s="260"/>
-      <c r="D8" s="260"/>
-      <c r="E8" s="260"/>
-      <c r="F8" s="260"/>
-      <c r="G8" s="260"/>
+      <c r="C8" s="264"/>
+      <c r="D8" s="264"/>
+      <c r="E8" s="264"/>
+      <c r="F8" s="264"/>
+      <c r="G8" s="264"/>
       <c r="H8" s="161"/>
       <c r="I8" s="156"/>
     </row>
@@ -8987,14 +8987,14 @@
     </row>
     <row r="10" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A10" s="154"/>
-      <c r="B10" s="261" t="s">
+      <c r="B10" s="265" t="s">
         <v>774</v>
       </c>
-      <c r="C10" s="261"/>
-      <c r="D10" s="261"/>
-      <c r="E10" s="261"/>
-      <c r="F10" s="261"/>
-      <c r="G10" s="261"/>
+      <c r="C10" s="265"/>
+      <c r="D10" s="265"/>
+      <c r="E10" s="265"/>
+      <c r="F10" s="265"/>
+      <c r="G10" s="265"/>
       <c r="H10" s="156"/>
       <c r="I10" s="156"/>
     </row>
@@ -9002,10 +9002,10 @@
       <c r="A11" s="154"/>
       <c r="B11" s="173"/>
       <c r="C11" s="173"/>
-      <c r="D11" s="261"/>
-      <c r="E11" s="261"/>
-      <c r="F11" s="261"/>
-      <c r="G11" s="261"/>
+      <c r="D11" s="265"/>
+      <c r="E11" s="265"/>
+      <c r="F11" s="265"/>
+      <c r="G11" s="265"/>
       <c r="H11" s="156"/>
       <c r="I11" s="156"/>
     </row>
@@ -9078,23 +9078,23 @@
     </row>
     <row r="17" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A17" s="154"/>
-      <c r="B17" s="263" t="s">
+      <c r="B17" s="259" t="s">
         <v>712</v>
       </c>
-      <c r="C17" s="263"/>
-      <c r="D17" s="263"/>
-      <c r="E17" s="263"/>
-      <c r="F17" s="263"/>
-      <c r="G17" s="263"/>
+      <c r="C17" s="259"/>
+      <c r="D17" s="259"/>
+      <c r="E17" s="259"/>
+      <c r="F17" s="259"/>
+      <c r="G17" s="259"/>
       <c r="H17" s="161"/>
       <c r="I17" s="156"/>
     </row>
     <row r="18" spans="1:9" s="160" customFormat="1">
       <c r="A18" s="159"/>
-      <c r="B18" s="264" t="s">
+      <c r="B18" s="260" t="s">
         <v>713</v>
       </c>
-      <c r="C18" s="264"/>
+      <c r="C18" s="260"/>
       <c r="D18" s="180" t="s">
         <v>714</v>
       </c>
@@ -9112,10 +9112,10 @@
     </row>
     <row r="19" spans="1:9" s="160" customFormat="1">
       <c r="A19" s="159"/>
-      <c r="B19" s="265" t="s">
+      <c r="B19" s="261" t="s">
         <v>718</v>
       </c>
-      <c r="C19" s="265"/>
+      <c r="C19" s="261"/>
       <c r="D19" s="166" t="s">
         <v>719</v>
       </c>
@@ -9154,10 +9154,10 @@
     </row>
     <row r="21" spans="1:9" s="160" customFormat="1">
       <c r="A21" s="159"/>
-      <c r="B21" s="262" t="s">
+      <c r="B21" s="258" t="s">
         <v>721</v>
       </c>
-      <c r="C21" s="262"/>
+      <c r="C21" s="258"/>
       <c r="D21" s="167" t="s">
         <v>722</v>
       </c>
@@ -9175,10 +9175,10 @@
     </row>
     <row r="22" spans="1:9" s="160" customFormat="1" ht="25.5">
       <c r="A22" s="159"/>
-      <c r="B22" s="262" t="s">
+      <c r="B22" s="258" t="s">
         <v>725</v>
       </c>
-      <c r="C22" s="262"/>
+      <c r="C22" s="258"/>
       <c r="D22" s="167" t="s">
         <v>726</v>
       </c>
@@ -9292,6 +9292,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="D11:G11"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="B21:C21"/>
@@ -9300,12 +9306,6 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F19" r:id="rId1"/>
@@ -13393,7 +13393,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" style="4" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" style="4" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="12" customWidth="1"/>
     <col min="3" max="3" width="51.7109375" style="4" customWidth="1"/>
     <col min="4" max="4" width="33.7109375" style="8" customWidth="1"/>

</xml_diff>

<commit_message>
Add 14 new crops
</commit_message>
<xml_diff>
--- a/src/main/dart/web/LCI-Database_Data-collection_Crop_v1.xlsx
+++ b/src/main/dart/web/LCI-Database_Data-collection_Crop_v1.xlsx
@@ -17,16 +17,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'User Guidance'!$B$2:$E$229</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2342" uniqueCount="975">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2356" uniqueCount="989">
   <si>
     <t>Country</t>
   </si>
@@ -3252,6 +3247,48 @@
   </si>
   <si>
     <t>Is responsible for all the modelling and scientific aspects of the tool</t>
+  </si>
+  <si>
+    <t>Bell pepper</t>
+  </si>
+  <si>
+    <t>Cabbage</t>
+  </si>
+  <si>
+    <t>Cashew</t>
+  </si>
+  <si>
+    <t>Cassava</t>
+  </si>
+  <si>
+    <t>Chilli</t>
+  </si>
+  <si>
+    <t>Cotton</t>
+  </si>
+  <si>
+    <t>Eggplant</t>
+  </si>
+  <si>
+    <t>Flax</t>
+  </si>
+  <si>
+    <t>Grape</t>
+  </si>
+  <si>
+    <t>Guar</t>
+  </si>
+  <si>
+    <t>Hemp</t>
+  </si>
+  <si>
+    <t>Lentil</t>
+  </si>
+  <si>
+    <t>Mango</t>
+  </si>
+  <si>
+    <t>Mulberry</t>
   </si>
 </sst>
 </file>
@@ -5175,7 +5212,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="271">
+  <cellXfs count="273">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -5870,6 +5907,18 @@
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -5882,18 +5931,6 @@
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5909,6 +5946,8 @@
     <xf numFmtId="0" fontId="9" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="613">
     <cellStyle name="(min) Duizend,0" xfId="4"/>
@@ -8045,7 +8084,7 @@
   <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:G6"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
@@ -8108,25 +8147,25 @@
     </row>
     <row r="5" spans="1:9" s="160" customFormat="1" ht="54.75" customHeight="1">
       <c r="A5" s="159"/>
-      <c r="B5" s="262"/>
-      <c r="C5" s="262"/>
-      <c r="D5" s="262"/>
-      <c r="E5" s="262"/>
-      <c r="F5" s="262"/>
-      <c r="G5" s="262"/>
+      <c r="B5" s="258"/>
+      <c r="C5" s="258"/>
+      <c r="D5" s="258"/>
+      <c r="E5" s="258"/>
+      <c r="F5" s="258"/>
+      <c r="G5" s="258"/>
       <c r="H5" s="156"/>
       <c r="I5" s="156"/>
     </row>
     <row r="6" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A6" s="154"/>
-      <c r="B6" s="263" t="s">
+      <c r="B6" s="259" t="s">
         <v>973</v>
       </c>
-      <c r="C6" s="263"/>
-      <c r="D6" s="263"/>
-      <c r="E6" s="263"/>
-      <c r="F6" s="263"/>
-      <c r="G6" s="263"/>
+      <c r="C6" s="259"/>
+      <c r="D6" s="259"/>
+      <c r="E6" s="259"/>
+      <c r="F6" s="259"/>
+      <c r="G6" s="259"/>
       <c r="H6" s="156"/>
       <c r="I6" s="156"/>
     </row>
@@ -8141,16 +8180,16 @@
       <c r="H7" s="156"/>
       <c r="I7" s="156"/>
     </row>
-    <row r="8" spans="1:9" s="157" customFormat="1" ht="15.95">
+    <row r="8" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A8" s="154"/>
-      <c r="B8" s="264" t="s">
+      <c r="B8" s="260" t="s">
         <v>708</v>
       </c>
-      <c r="C8" s="264"/>
-      <c r="D8" s="264"/>
-      <c r="E8" s="264"/>
-      <c r="F8" s="264"/>
-      <c r="G8" s="264"/>
+      <c r="C8" s="260"/>
+      <c r="D8" s="260"/>
+      <c r="E8" s="260"/>
+      <c r="F8" s="260"/>
+      <c r="G8" s="260"/>
       <c r="H8" s="161"/>
       <c r="I8" s="156"/>
     </row>
@@ -8167,14 +8206,14 @@
     </row>
     <row r="10" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A10" s="154"/>
-      <c r="B10" s="265" t="s">
+      <c r="B10" s="261" t="s">
         <v>772</v>
       </c>
-      <c r="C10" s="265"/>
-      <c r="D10" s="265"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="265"/>
-      <c r="G10" s="265"/>
+      <c r="C10" s="261"/>
+      <c r="D10" s="261"/>
+      <c r="E10" s="261"/>
+      <c r="F10" s="261"/>
+      <c r="G10" s="261"/>
       <c r="H10" s="156"/>
       <c r="I10" s="156"/>
     </row>
@@ -8182,10 +8221,10 @@
       <c r="A11" s="154"/>
       <c r="B11" s="173"/>
       <c r="C11" s="173"/>
-      <c r="D11" s="265"/>
-      <c r="E11" s="265"/>
-      <c r="F11" s="265"/>
-      <c r="G11" s="265"/>
+      <c r="D11" s="261"/>
+      <c r="E11" s="261"/>
+      <c r="F11" s="261"/>
+      <c r="G11" s="261"/>
       <c r="H11" s="156"/>
       <c r="I11" s="156"/>
     </row>
@@ -8256,25 +8295,25 @@
       <c r="H16" s="156"/>
       <c r="I16" s="156"/>
     </row>
-    <row r="17" spans="1:9" s="157" customFormat="1" ht="15.95">
+    <row r="17" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A17" s="154"/>
-      <c r="B17" s="259" t="s">
+      <c r="B17" s="263" t="s">
         <v>711</v>
       </c>
-      <c r="C17" s="259"/>
-      <c r="D17" s="259"/>
-      <c r="E17" s="259"/>
-      <c r="F17" s="259"/>
-      <c r="G17" s="259"/>
+      <c r="C17" s="263"/>
+      <c r="D17" s="263"/>
+      <c r="E17" s="263"/>
+      <c r="F17" s="263"/>
+      <c r="G17" s="263"/>
       <c r="H17" s="161"/>
       <c r="I17" s="156"/>
     </row>
-    <row r="18" spans="1:9" s="160" customFormat="1" ht="14.1">
+    <row r="18" spans="1:9" s="160" customFormat="1">
       <c r="A18" s="159"/>
-      <c r="B18" s="260" t="s">
+      <c r="B18" s="264" t="s">
         <v>712</v>
       </c>
-      <c r="C18" s="260"/>
+      <c r="C18" s="264"/>
       <c r="D18" s="180" t="s">
         <v>713</v>
       </c>
@@ -8290,12 +8329,12 @@
       <c r="H18" s="156"/>
       <c r="I18" s="156"/>
     </row>
-    <row r="19" spans="1:9" s="160" customFormat="1" ht="14.1">
+    <row r="19" spans="1:9" s="160" customFormat="1">
       <c r="A19" s="159"/>
-      <c r="B19" s="261" t="s">
+      <c r="B19" s="265" t="s">
         <v>717</v>
       </c>
-      <c r="C19" s="261"/>
+      <c r="C19" s="265"/>
       <c r="D19" s="166" t="s">
         <v>718</v>
       </c>
@@ -8334,10 +8373,10 @@
     </row>
     <row r="21" spans="1:9" s="160" customFormat="1">
       <c r="A21" s="159"/>
-      <c r="B21" s="258" t="s">
+      <c r="B21" s="262" t="s">
         <v>720</v>
       </c>
-      <c r="C21" s="258"/>
+      <c r="C21" s="262"/>
       <c r="D21" s="167" t="s">
         <v>721</v>
       </c>
@@ -8355,10 +8394,10 @@
     </row>
     <row r="22" spans="1:9" s="160" customFormat="1" ht="25.5">
       <c r="A22" s="159"/>
-      <c r="B22" s="258" t="s">
+      <c r="B22" s="262" t="s">
         <v>724</v>
       </c>
-      <c r="C22" s="258"/>
+      <c r="C22" s="262"/>
       <c r="D22" s="167" t="s">
         <v>725</v>
       </c>
@@ -8374,7 +8413,7 @@
       <c r="H22" s="156"/>
       <c r="I22" s="156"/>
     </row>
-    <row r="23" spans="1:9" s="157" customFormat="1" ht="14.1">
+    <row r="23" spans="1:9" s="157" customFormat="1">
       <c r="A23" s="154"/>
       <c r="B23" s="177"/>
       <c r="C23" s="177"/>
@@ -8385,7 +8424,7 @@
       <c r="H23" s="156"/>
       <c r="I23" s="156"/>
     </row>
-    <row r="24" spans="1:9" ht="14.1">
+    <row r="24" spans="1:9">
       <c r="B24" s="172"/>
       <c r="C24" s="172"/>
       <c r="D24" s="178"/>
@@ -8393,7 +8432,7 @@
       <c r="F24" s="178"/>
       <c r="G24" s="178"/>
     </row>
-    <row r="25" spans="1:9" s="165" customFormat="1" ht="15.95">
+    <row r="25" spans="1:9" s="165" customFormat="1" ht="15.75">
       <c r="A25" s="164"/>
       <c r="B25" s="171" t="s">
         <v>727</v>
@@ -8426,7 +8465,7 @@
       <c r="F27" s="178"/>
       <c r="G27" s="178"/>
     </row>
-    <row r="28" spans="1:9" s="165" customFormat="1" ht="14.1">
+    <row r="28" spans="1:9" s="165" customFormat="1">
       <c r="A28" s="164"/>
       <c r="B28" s="172" t="s">
         <v>729</v>
@@ -8437,7 +8476,7 @@
       <c r="F28" s="178"/>
       <c r="G28" s="178"/>
     </row>
-    <row r="29" spans="1:9" s="165" customFormat="1" ht="14.1">
+    <row r="29" spans="1:9" s="165" customFormat="1">
       <c r="A29" s="164"/>
       <c r="B29" s="172" t="s">
         <v>730</v>
@@ -8448,7 +8487,7 @@
       <c r="F29" s="178"/>
       <c r="G29" s="178"/>
     </row>
-    <row r="30" spans="1:9" s="165" customFormat="1" ht="14.1">
+    <row r="30" spans="1:9" s="165" customFormat="1">
       <c r="A30" s="164"/>
       <c r="B30" s="172" t="s">
         <v>731</v>
@@ -8459,7 +8498,7 @@
       <c r="F30" s="178"/>
       <c r="G30" s="178"/>
     </row>
-    <row r="31" spans="1:9" s="165" customFormat="1" ht="14.1">
+    <row r="31" spans="1:9" s="165" customFormat="1">
       <c r="A31" s="164"/>
       <c r="B31" s="172" t="s">
         <v>732</v>
@@ -8472,12 +8511,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="D11:G11"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="B21:C21"/>
@@ -8486,6 +8519,12 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <phoneticPr fontId="83" type="noConversion"/>
   <hyperlinks>
@@ -8509,8 +8548,8 @@
   <sheetViews>
     <sheetView topLeftCell="B2" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B35" sqref="B35"/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -12560,7 +12599,7 @@
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -17239,7 +17278,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$I$2:$I$36</xm:f>
+            <xm:f>Lists!$I$2:$I$50</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
@@ -17268,10 +17307,10 @@
   </sheetPr>
   <dimension ref="A1:O141"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B35" sqref="B35"/>
-      <selection pane="bottomLeft" activeCell="G113" sqref="G113"/>
+      <selection pane="bottomLeft" activeCell="I50" sqref="I50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17279,7 +17318,7 @@
     <col min="1" max="15" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="234" customFormat="1">
+    <row r="1" spans="1:15" s="234" customFormat="1" ht="30">
       <c r="A1" s="233" t="s">
         <v>117</v>
       </c>
@@ -17326,7 +17365,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="2" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>367</v>
       </c>
@@ -17373,7 +17412,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="3" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A3" s="1" t="s">
         <v>124</v>
       </c>
@@ -17398,7 +17437,7 @@
       <c r="H3" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="272" t="s">
         <v>172</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -17420,7 +17459,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="4" spans="1:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="A4" s="1" t="s">
         <v>125</v>
       </c>
@@ -17445,7 +17484,7 @@
       <c r="H4" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="272" t="s">
         <v>179</v>
       </c>
       <c r="J4" s="1" t="s">
@@ -17467,7 +17506,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="5" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A5" s="1" t="s">
         <v>126</v>
       </c>
@@ -17492,7 +17531,7 @@
       <c r="H5" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="272" t="s">
         <v>185</v>
       </c>
       <c r="J5" s="1" t="s">
@@ -17514,7 +17553,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="6" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="6" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A6" s="1" t="s">
         <v>127</v>
       </c>
@@ -17536,7 +17575,7 @@
       <c r="H6" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="272" t="s">
         <v>190</v>
       </c>
       <c r="J6" s="1" t="s">
@@ -17555,7 +17594,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="7" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A7" s="1" t="s">
         <v>128</v>
       </c>
@@ -17574,7 +17613,7 @@
       <c r="H7" s="9" t="s">
         <v>913</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="272" t="s">
         <v>193</v>
       </c>
       <c r="J7" s="1" t="s">
@@ -17593,7 +17632,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="8" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A8" s="1" t="s">
         <v>129</v>
       </c>
@@ -17603,8 +17642,8 @@
       <c r="G8" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>197</v>
+      <c r="I8" s="271" t="s">
+        <v>975</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>60</v>
@@ -17622,15 +17661,15 @@
         <v>953</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="9" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="D9" s="1" t="s">
         <v>198</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>200</v>
+      <c r="I9" s="271" t="s">
+        <v>976</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>61</v>
@@ -17648,15 +17687,15 @@
         <v>579</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="10" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="D10" s="1" t="s">
         <v>201</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>203</v>
+      <c r="I10" s="272" t="s">
+        <v>197</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>62</v>
@@ -17674,15 +17713,15 @@
         <v>580</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="1" customFormat="1" ht="27.95" thickBot="1">
+    <row r="11" spans="1:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="D11" s="1" t="s">
         <v>204</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>206</v>
+      <c r="I11" s="271" t="s">
+        <v>977</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>63</v>
@@ -17700,15 +17739,15 @@
         <v>581</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="12" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="D12" s="1" t="s">
         <v>913</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>231</v>
+      <c r="I12" s="271" t="s">
+        <v>978</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>59</v>
@@ -17723,12 +17762,12 @@
         <v>582</v>
       </c>
     </row>
-    <row r="13" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="13" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="G13" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>209</v>
+      <c r="I13" s="271" t="s">
+        <v>979</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>65</v>
@@ -17743,12 +17782,12 @@
         <v>583</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="14" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="G14" s="9" t="s">
         <v>913</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>232</v>
+      <c r="I14" s="272" t="s">
+        <v>200</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>67</v>
@@ -17763,9 +17802,9 @@
         <v>584</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I15" s="1" t="s">
-        <v>210</v>
+    <row r="15" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I15" s="272" t="s">
+        <v>203</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>68</v>
@@ -17780,9 +17819,9 @@
         <v>952</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I16" s="1" t="s">
-        <v>211</v>
+    <row r="16" spans="1:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I16" s="272" t="s">
+        <v>206</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>64</v>
@@ -17797,9 +17836,9 @@
         <v>650</v>
       </c>
     </row>
-    <row r="17" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I17" s="1" t="s">
-        <v>212</v>
+    <row r="17" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I17" s="271" t="s">
+        <v>980</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>69</v>
@@ -17814,9 +17853,9 @@
         <v>585</v>
       </c>
     </row>
-    <row r="18" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I18" s="1" t="s">
-        <v>213</v>
+    <row r="18" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I18" s="271" t="s">
+        <v>981</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>70</v>
@@ -17831,9 +17870,9 @@
         <v>586</v>
       </c>
     </row>
-    <row r="19" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I19" s="1" t="s">
-        <v>214</v>
+    <row r="19" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="I19" s="271" t="s">
+        <v>982</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>73</v>
@@ -17848,9 +17887,9 @@
         <v>587</v>
       </c>
     </row>
-    <row r="20" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I20" s="1" t="s">
-        <v>215</v>
+    <row r="20" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I20" s="271" t="s">
+        <v>983</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>71</v>
@@ -17865,9 +17904,9 @@
         <v>588</v>
       </c>
     </row>
-    <row r="21" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I21" s="1" t="s">
-        <v>233</v>
+    <row r="21" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I21" s="271" t="s">
+        <v>984</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>72</v>
@@ -17882,9 +17921,9 @@
         <v>589</v>
       </c>
     </row>
-    <row r="22" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I22" s="1" t="s">
-        <v>216</v>
+    <row r="22" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I22" s="271" t="s">
+        <v>985</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>74</v>
@@ -17899,9 +17938,9 @@
         <v>590</v>
       </c>
     </row>
-    <row r="23" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I23" s="1" t="s">
-        <v>217</v>
+    <row r="23" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I23" s="272" t="s">
+        <v>231</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>75</v>
@@ -17916,9 +17955,9 @@
         <v>651</v>
       </c>
     </row>
-    <row r="24" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I24" s="1" t="s">
-        <v>218</v>
+    <row r="24" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I24" s="271" t="s">
+        <v>986</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>77</v>
@@ -17933,9 +17972,9 @@
         <v>954</v>
       </c>
     </row>
-    <row r="25" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I25" s="1" t="s">
-        <v>219</v>
+    <row r="25" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I25" s="272" t="s">
+        <v>209</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>78</v>
@@ -17950,9 +17989,9 @@
         <v>591</v>
       </c>
     </row>
-    <row r="26" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I26" s="1" t="s">
-        <v>220</v>
+    <row r="26" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I26" s="272" t="s">
+        <v>232</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>79</v>
@@ -17967,9 +18006,9 @@
         <v>592</v>
       </c>
     </row>
-    <row r="27" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I27" s="1" t="s">
-        <v>221</v>
+    <row r="27" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I27" s="272" t="s">
+        <v>210</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>80</v>
@@ -17984,9 +18023,9 @@
         <v>593</v>
       </c>
     </row>
-    <row r="28" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I28" s="1" t="s">
-        <v>222</v>
+    <row r="28" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I28" s="271" t="s">
+        <v>987</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>81</v>
@@ -18001,9 +18040,9 @@
         <v>593</v>
       </c>
     </row>
-    <row r="29" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I29" s="1" t="s">
-        <v>223</v>
+    <row r="29" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I29" s="272" t="s">
+        <v>211</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>82</v>
@@ -18018,9 +18057,9 @@
         <v>594</v>
       </c>
     </row>
-    <row r="30" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I30" s="1" t="s">
-        <v>228</v>
+    <row r="30" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I30" s="271" t="s">
+        <v>988</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>83</v>
@@ -18035,9 +18074,9 @@
         <v>595</v>
       </c>
     </row>
-    <row r="31" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I31" s="1" t="s">
-        <v>229</v>
+    <row r="31" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I31" s="272" t="s">
+        <v>212</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>89</v>
@@ -18052,9 +18091,9 @@
         <v>652</v>
       </c>
     </row>
-    <row r="32" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I32" s="1" t="s">
-        <v>224</v>
+    <row r="32" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="I32" s="272" t="s">
+        <v>213</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>66</v>
@@ -18069,9 +18108,9 @@
         <v>596</v>
       </c>
     </row>
-    <row r="33" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I33" s="1" t="s">
-        <v>230</v>
+    <row r="33" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I33" s="272" t="s">
+        <v>214</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>76</v>
@@ -18086,9 +18125,9 @@
         <v>955</v>
       </c>
     </row>
-    <row r="34" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I34" s="1" t="s">
-        <v>225</v>
+    <row r="34" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I34" s="272" t="s">
+        <v>215</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>54</v>
@@ -18103,9 +18142,9 @@
         <v>653</v>
       </c>
     </row>
-    <row r="35" spans="9:15" s="1" customFormat="1" ht="27.95" thickBot="1">
-      <c r="I35" s="1" t="s">
-        <v>226</v>
+    <row r="35" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="I35" s="272" t="s">
+        <v>233</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>84</v>
@@ -18120,9 +18159,9 @@
         <v>597</v>
       </c>
     </row>
-    <row r="36" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
-      <c r="I36" s="1" t="s">
-        <v>227</v>
+    <row r="36" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I36" s="272" t="s">
+        <v>216</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>85</v>
@@ -18137,7 +18176,10 @@
         <v>598</v>
       </c>
     </row>
-    <row r="37" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="37" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I37" s="272" t="s">
+        <v>217</v>
+      </c>
       <c r="J37" s="1" t="s">
         <v>86</v>
       </c>
@@ -18151,7 +18193,10 @@
         <v>956</v>
       </c>
     </row>
-    <row r="38" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="38" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I38" s="272" t="s">
+        <v>218</v>
+      </c>
       <c r="J38" s="1" t="s">
         <v>87</v>
       </c>
@@ -18165,7 +18210,10 @@
         <v>599</v>
       </c>
     </row>
-    <row r="39" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="39" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I39" s="272" t="s">
+        <v>219</v>
+      </c>
       <c r="J39" s="1" t="s">
         <v>88</v>
       </c>
@@ -18179,7 +18227,10 @@
         <v>600</v>
       </c>
     </row>
-    <row r="40" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="40" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I40" s="272" t="s">
+        <v>220</v>
+      </c>
       <c r="M40" s="256" t="s">
         <v>402</v>
       </c>
@@ -18190,7 +18241,10 @@
         <v>601</v>
       </c>
     </row>
-    <row r="41" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="41" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I41" s="272" t="s">
+        <v>221</v>
+      </c>
       <c r="M41" s="256" t="s">
         <v>919</v>
       </c>
@@ -18201,7 +18255,10 @@
         <v>602</v>
       </c>
     </row>
-    <row r="42" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="42" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I42" s="272" t="s">
+        <v>222</v>
+      </c>
       <c r="M42" s="256" t="s">
         <v>404</v>
       </c>
@@ -18212,7 +18269,10 @@
         <v>603</v>
       </c>
     </row>
-    <row r="43" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="43" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I43" s="272" t="s">
+        <v>223</v>
+      </c>
       <c r="M43" s="256" t="s">
         <v>405</v>
       </c>
@@ -18223,7 +18283,10 @@
         <v>604</v>
       </c>
     </row>
-    <row r="44" spans="9:15" s="1" customFormat="1" ht="27.95" thickBot="1">
+    <row r="44" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="I44" s="272" t="s">
+        <v>228</v>
+      </c>
       <c r="M44" s="256" t="s">
         <v>406</v>
       </c>
@@ -18234,7 +18297,10 @@
         <v>605</v>
       </c>
     </row>
-    <row r="45" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="45" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I45" s="272" t="s">
+        <v>229</v>
+      </c>
       <c r="M45" s="256" t="s">
         <v>407</v>
       </c>
@@ -18245,7 +18311,10 @@
         <v>606</v>
       </c>
     </row>
-    <row r="46" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="46" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I46" s="272" t="s">
+        <v>224</v>
+      </c>
       <c r="M46" s="256" t="s">
         <v>408</v>
       </c>
@@ -18256,7 +18325,10 @@
         <v>607</v>
       </c>
     </row>
-    <row r="47" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="47" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I47" s="272" t="s">
+        <v>230</v>
+      </c>
       <c r="M47" s="256" t="s">
         <v>409</v>
       </c>
@@ -18267,7 +18339,10 @@
         <v>608</v>
       </c>
     </row>
-    <row r="48" spans="9:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="48" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I48" s="272" t="s">
+        <v>225</v>
+      </c>
       <c r="M48" s="256" t="s">
         <v>410</v>
       </c>
@@ -18278,7 +18353,10 @@
         <v>957</v>
       </c>
     </row>
-    <row r="49" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="49" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I49" s="272" t="s">
+        <v>226</v>
+      </c>
       <c r="M49" s="256" t="s">
         <v>411</v>
       </c>
@@ -18289,7 +18367,10 @@
         <v>958</v>
       </c>
     </row>
-    <row r="50" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="50" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I50" s="272" t="s">
+        <v>227</v>
+      </c>
       <c r="M50" s="256" t="s">
         <v>403</v>
       </c>
@@ -18300,7 +18381,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="51" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="51" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M51" s="256" t="s">
         <v>412</v>
       </c>
@@ -18311,7 +18392,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="52" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="52" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M52" s="256" t="s">
         <v>413</v>
       </c>
@@ -18322,7 +18403,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="53" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="53" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M53" s="256" t="s">
         <v>414</v>
       </c>
@@ -18333,7 +18414,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="54" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="54" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M54" s="256" t="s">
         <v>415</v>
       </c>
@@ -18344,7 +18425,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="55" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="55" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M55" s="256" t="s">
         <v>924</v>
       </c>
@@ -18355,7 +18436,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="56" spans="13:15" s="1" customFormat="1" ht="27.95" thickBot="1">
+    <row r="56" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M56" s="256" t="s">
         <v>925</v>
       </c>
@@ -18366,7 +18447,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="57" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="57" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M57" s="256" t="s">
         <v>416</v>
       </c>
@@ -18377,7 +18458,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="58" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="58" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M58" s="256" t="s">
         <v>417</v>
       </c>
@@ -18388,7 +18469,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="59" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="59" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M59" s="256" t="s">
         <v>418</v>
       </c>
@@ -18399,7 +18480,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="60" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="60" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M60" s="256" t="s">
         <v>419</v>
       </c>
@@ -18410,7 +18491,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="61" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="61" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M61" s="256" t="s">
         <v>420</v>
       </c>
@@ -18421,7 +18502,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="62" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="62" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M62" s="256" t="s">
         <v>421</v>
       </c>
@@ -18432,7 +18513,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="63" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="63" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M63" s="256" t="s">
         <v>926</v>
       </c>
@@ -18443,7 +18524,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="64" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="64" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M64" s="256" t="s">
         <v>422</v>
       </c>
@@ -18454,7 +18535,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="65" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="65" spans="13:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M65" s="256" t="s">
         <v>927</v>
       </c>
@@ -18465,7 +18546,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="66" spans="13:15" s="1" customFormat="1" ht="15.95" thickBot="1">
+    <row r="66" spans="13:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M66" s="256" t="s">
         <v>423</v>
       </c>
@@ -18476,7 +18557,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="67" spans="13:15" ht="15.95" thickBot="1">
+    <row r="67" spans="13:15" ht="15.75" thickBot="1">
       <c r="M67" s="256" t="s">
         <v>424</v>
       </c>
@@ -18487,7 +18568,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="68" spans="13:15" ht="27.95" thickBot="1">
+    <row r="68" spans="13:15" ht="27" thickBot="1">
       <c r="M68" s="256" t="s">
         <v>425</v>
       </c>
@@ -18498,7 +18579,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="69" spans="13:15" ht="15.95" thickBot="1">
+    <row r="69" spans="13:15" ht="15.75" thickBot="1">
       <c r="M69" s="256" t="s">
         <v>929</v>
       </c>
@@ -18509,7 +18590,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="70" spans="13:15" ht="15.95" thickBot="1">
+    <row r="70" spans="13:15" ht="15.75" thickBot="1">
       <c r="M70" s="256" t="s">
         <v>930</v>
       </c>
@@ -18520,7 +18601,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="71" spans="13:15" ht="15.95" thickBot="1">
+    <row r="71" spans="13:15" ht="15.75" thickBot="1">
       <c r="M71" s="256" t="s">
         <v>426</v>
       </c>
@@ -18531,7 +18612,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="72" spans="13:15" ht="15.95" thickBot="1">
+    <row r="72" spans="13:15" ht="15.75" thickBot="1">
       <c r="M72" s="256" t="s">
         <v>427</v>
       </c>
@@ -18542,7 +18623,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="73" spans="13:15" ht="27.95" thickBot="1">
+    <row r="73" spans="13:15" ht="27" thickBot="1">
       <c r="M73" s="256" t="s">
         <v>428</v>
       </c>
@@ -18553,7 +18634,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="74" spans="13:15" ht="15.95" thickBot="1">
+    <row r="74" spans="13:15" ht="15.75" thickBot="1">
       <c r="M74" s="256" t="s">
         <v>429</v>
       </c>
@@ -18564,7 +18645,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="75" spans="13:15" ht="15.95" thickBot="1">
+    <row r="75" spans="13:15" ht="15.75" thickBot="1">
       <c r="M75" s="256" t="s">
         <v>931</v>
       </c>
@@ -18575,7 +18656,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="76" spans="13:15" ht="15.95" thickBot="1">
+    <row r="76" spans="13:15" ht="15.75" thickBot="1">
       <c r="M76" s="256" t="s">
         <v>431</v>
       </c>
@@ -18586,7 +18667,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="77" spans="13:15" ht="15.95" thickBot="1">
+    <row r="77" spans="13:15" ht="15.75" thickBot="1">
       <c r="M77" s="256" t="s">
         <v>430</v>
       </c>
@@ -18597,7 +18678,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="78" spans="13:15" ht="15.95" thickBot="1">
+    <row r="78" spans="13:15" ht="15.75" thickBot="1">
       <c r="M78" s="256" t="s">
         <v>432</v>
       </c>
@@ -18608,7 +18689,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="79" spans="13:15" ht="27.95" thickBot="1">
+    <row r="79" spans="13:15" ht="27" thickBot="1">
       <c r="M79" s="256" t="s">
         <v>433</v>
       </c>
@@ -18619,7 +18700,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="80" spans="13:15" ht="15.95" thickBot="1">
+    <row r="80" spans="13:15" ht="15.75" thickBot="1">
       <c r="M80" s="256" t="s">
         <v>434</v>
       </c>
@@ -18630,7 +18711,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="81" spans="13:15" ht="15.95" thickBot="1">
+    <row r="81" spans="13:15" ht="15.75" thickBot="1">
       <c r="M81" s="256" t="s">
         <v>435</v>
       </c>
@@ -18641,7 +18722,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="82" spans="13:15" ht="15.95" thickBot="1">
+    <row r="82" spans="13:15" ht="15.75" thickBot="1">
       <c r="M82" s="256" t="s">
         <v>436</v>
       </c>
@@ -18652,7 +18733,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="83" spans="13:15" ht="15.95" thickBot="1">
+    <row r="83" spans="13:15" ht="15.75" thickBot="1">
       <c r="M83" s="256" t="s">
         <v>437</v>
       </c>
@@ -18663,7 +18744,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="84" spans="13:15" ht="15.95" thickBot="1">
+    <row r="84" spans="13:15" ht="15.75" thickBot="1">
       <c r="M84" s="256" t="s">
         <v>438</v>
       </c>
@@ -18674,7 +18755,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="85" spans="13:15" ht="15.95" thickBot="1">
+    <row r="85" spans="13:15" ht="15.75" thickBot="1">
       <c r="M85" s="256" t="s">
         <v>439</v>
       </c>
@@ -18685,7 +18766,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="86" spans="13:15" ht="15.95" thickBot="1">
+    <row r="86" spans="13:15" ht="15.75" thickBot="1">
       <c r="M86" s="256" t="s">
         <v>440</v>
       </c>
@@ -18696,7 +18777,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="87" spans="13:15" ht="15.95" thickBot="1">
+    <row r="87" spans="13:15" ht="15.75" thickBot="1">
       <c r="M87" s="256" t="s">
         <v>441</v>
       </c>
@@ -18707,7 +18788,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="88" spans="13:15" ht="15.95" thickBot="1">
+    <row r="88" spans="13:15" ht="15.75" thickBot="1">
       <c r="M88" s="256" t="s">
         <v>442</v>
       </c>
@@ -18718,7 +18799,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="89" spans="13:15" ht="15.95" thickBot="1">
+    <row r="89" spans="13:15" ht="15.75" thickBot="1">
       <c r="M89" s="256" t="s">
         <v>443</v>
       </c>
@@ -18729,7 +18810,7 @@
         <v>967</v>
       </c>
     </row>
-    <row r="90" spans="13:15" ht="15.95" thickBot="1">
+    <row r="90" spans="13:15" ht="15.75" thickBot="1">
       <c r="M90" s="256" t="s">
         <v>444</v>
       </c>
@@ -18740,7 +18821,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="91" spans="13:15" ht="15.95" thickBot="1">
+    <row r="91" spans="13:15" ht="15.75" thickBot="1">
       <c r="M91" s="256" t="s">
         <v>445</v>
       </c>
@@ -18751,7 +18832,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="92" spans="13:15" ht="15.95" thickBot="1">
+    <row r="92" spans="13:15" ht="15.75" thickBot="1">
       <c r="M92" s="256" t="s">
         <v>446</v>
       </c>
@@ -18762,7 +18843,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="93" spans="13:15" ht="15.95" thickBot="1">
+    <row r="93" spans="13:15" ht="15.75" thickBot="1">
       <c r="M93" s="256" t="s">
         <v>934</v>
       </c>
@@ -18773,7 +18854,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="94" spans="13:15" ht="15.95" thickBot="1">
+    <row r="94" spans="13:15" ht="15.75" thickBot="1">
       <c r="M94" s="256" t="s">
         <v>447</v>
       </c>
@@ -18784,7 +18865,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="95" spans="13:15" ht="15.95" thickBot="1">
+    <row r="95" spans="13:15" ht="15.75" thickBot="1">
       <c r="M95" s="256" t="s">
         <v>448</v>
       </c>
@@ -18795,7 +18876,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="96" spans="13:15" ht="15.95" thickBot="1">
+    <row r="96" spans="13:15" ht="15.75" thickBot="1">
       <c r="M96" s="256" t="s">
         <v>449</v>
       </c>
@@ -18806,7 +18887,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="97" spans="13:15" ht="15.95" thickBot="1">
+    <row r="97" spans="13:15" ht="15.75" thickBot="1">
       <c r="M97" s="256" t="s">
         <v>450</v>
       </c>
@@ -18817,7 +18898,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="98" spans="13:15" ht="15.95" thickBot="1">
+    <row r="98" spans="13:15" ht="15.75" thickBot="1">
       <c r="M98" s="256" t="s">
         <v>451</v>
       </c>
@@ -18828,7 +18909,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="99" spans="13:15" ht="15.95" thickBot="1">
+    <row r="99" spans="13:15" ht="15.75" thickBot="1">
       <c r="M99" s="256" t="s">
         <v>452</v>
       </c>
@@ -18839,7 +18920,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="100" spans="13:15" ht="15.95" thickBot="1">
+    <row r="100" spans="13:15" ht="15.75" thickBot="1">
       <c r="M100" s="256" t="s">
         <v>453</v>
       </c>
@@ -18850,7 +18931,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="101" spans="13:15" ht="15.95" thickBot="1">
+    <row r="101" spans="13:15" ht="15.75" thickBot="1">
       <c r="M101" s="256" t="s">
         <v>454</v>
       </c>
@@ -18861,7 +18942,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="102" spans="13:15" ht="15.95" thickBot="1">
+    <row r="102" spans="13:15" ht="15.75" thickBot="1">
       <c r="M102" s="256" t="s">
         <v>455</v>
       </c>
@@ -18872,7 +18953,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="103" spans="13:15" ht="15.95" thickBot="1">
+    <row r="103" spans="13:15" ht="27" thickBot="1">
       <c r="M103" s="256" t="s">
         <v>457</v>
       </c>
@@ -18883,7 +18964,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="104" spans="13:15" ht="15.95" thickBot="1">
+    <row r="104" spans="13:15" ht="15.75" thickBot="1">
       <c r="M104" s="256" t="s">
         <v>456</v>
       </c>
@@ -18891,7 +18972,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="105" spans="13:15" ht="15.95" thickBot="1">
+    <row r="105" spans="13:15" ht="15.75" thickBot="1">
       <c r="M105" s="256" t="s">
         <v>458</v>
       </c>
@@ -18899,7 +18980,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="106" spans="13:15" ht="15.95" thickBot="1">
+    <row r="106" spans="13:15" ht="15.75" thickBot="1">
       <c r="M106" s="256" t="s">
         <v>459</v>
       </c>
@@ -18907,7 +18988,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="107" spans="13:15" ht="15.95" thickBot="1">
+    <row r="107" spans="13:15" ht="27" thickBot="1">
       <c r="M107" s="256" t="s">
         <v>460</v>
       </c>
@@ -18915,157 +18996,157 @@
         <v>658</v>
       </c>
     </row>
-    <row r="108" spans="13:15" ht="15.95" thickBot="1">
+    <row r="108" spans="13:15" ht="15.75" thickBot="1">
       <c r="M108" s="256" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="109" spans="13:15" ht="15.95" thickBot="1">
+    <row r="109" spans="13:15" ht="15.75" thickBot="1">
       <c r="M109" s="256" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="110" spans="13:15" ht="15.95" thickBot="1">
+    <row r="110" spans="13:15" ht="15.75" thickBot="1">
       <c r="M110" s="256" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="111" spans="13:15" ht="15.95" thickBot="1">
+    <row r="111" spans="13:15" ht="15.75" thickBot="1">
       <c r="M111" s="256" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="112" spans="13:15" ht="15.95" thickBot="1">
+    <row r="112" spans="13:15" ht="15.75" thickBot="1">
       <c r="M112" s="256" t="s">
         <v>463</v>
       </c>
     </row>
-    <row r="113" spans="13:13" ht="15.95" thickBot="1">
+    <row r="113" spans="13:13" ht="15.75" thickBot="1">
       <c r="M113" s="256" t="s">
         <v>464</v>
       </c>
     </row>
-    <row r="114" spans="13:13" ht="27.95" thickBot="1">
+    <row r="114" spans="13:13" ht="27" thickBot="1">
       <c r="M114" s="256" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="115" spans="13:13" ht="15.95" thickBot="1">
+    <row r="115" spans="13:13" ht="15.75" thickBot="1">
       <c r="M115" s="256" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="116" spans="13:13" ht="15.95" thickBot="1">
+    <row r="116" spans="13:13" ht="15.75" thickBot="1">
       <c r="M116" s="256" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="117" spans="13:13" ht="15.95" thickBot="1">
+    <row r="117" spans="13:13" ht="15.75" thickBot="1">
       <c r="M117" s="256" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="118" spans="13:13" ht="15.95" thickBot="1">
+    <row r="118" spans="13:13" ht="15.75" thickBot="1">
       <c r="M118" s="256" t="s">
         <v>469</v>
       </c>
     </row>
-    <row r="119" spans="13:13" ht="15.95" thickBot="1">
+    <row r="119" spans="13:13" ht="15.75" thickBot="1">
       <c r="M119" s="256" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="120" spans="13:13" ht="15.95" thickBot="1">
+    <row r="120" spans="13:13" ht="15.75" thickBot="1">
       <c r="M120" s="256" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="121" spans="13:13" ht="15.95" thickBot="1">
+    <row r="121" spans="13:13" ht="15.75" thickBot="1">
       <c r="M121" s="256" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="122" spans="13:13" ht="15.95" thickBot="1">
+    <row r="122" spans="13:13" ht="15.75" thickBot="1">
       <c r="M122" s="256" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="123" spans="13:13" ht="15.95" thickBot="1">
+    <row r="123" spans="13:13" ht="15.75" thickBot="1">
       <c r="M123" s="256" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="124" spans="13:13" ht="15.95" thickBot="1">
+    <row r="124" spans="13:13" ht="15.75" thickBot="1">
       <c r="M124" s="256" t="s">
         <v>928</v>
       </c>
     </row>
-    <row r="125" spans="13:13" ht="15.95" thickBot="1">
+    <row r="125" spans="13:13" ht="15.75" thickBot="1">
       <c r="M125" s="256" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="126" spans="13:13" ht="15.95" thickBot="1">
+    <row r="126" spans="13:13" ht="15.75" thickBot="1">
       <c r="M126" s="256" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="127" spans="13:13" ht="15.95" thickBot="1">
+    <row r="127" spans="13:13" ht="15.75" thickBot="1">
       <c r="M127" s="256" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="128" spans="13:13" ht="15.95" thickBot="1">
+    <row r="128" spans="13:13" ht="15.75" thickBot="1">
       <c r="M128" s="256" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="129" spans="13:13" ht="15.95" thickBot="1">
+    <row r="129" spans="13:13" ht="15.75" thickBot="1">
       <c r="M129" s="256" t="s">
         <v>478</v>
       </c>
     </row>
-    <row r="130" spans="13:13" ht="15.95" thickBot="1">
+    <row r="130" spans="13:13" ht="15.75" thickBot="1">
       <c r="M130" s="256" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="131" spans="13:13" ht="15.95" thickBot="1">
+    <row r="131" spans="13:13" ht="15.75" thickBot="1">
       <c r="M131" s="256" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="132" spans="13:13" ht="15.95" thickBot="1">
+    <row r="132" spans="13:13" ht="15.75" thickBot="1">
       <c r="M132" s="256" t="s">
         <v>480</v>
       </c>
     </row>
-    <row r="133" spans="13:13" ht="15.95" thickBot="1">
+    <row r="133" spans="13:13" ht="15.75" thickBot="1">
       <c r="M133" s="256" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="134" spans="13:13" ht="15.95" thickBot="1">
+    <row r="134" spans="13:13" ht="15.75" thickBot="1">
       <c r="M134" s="256" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="135" spans="13:13" ht="15.95" thickBot="1">
+    <row r="135" spans="13:13" ht="15.75" thickBot="1">
       <c r="M135" s="256" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="136" spans="13:13" ht="15.95" thickBot="1">
+    <row r="136" spans="13:13" ht="15.75" thickBot="1">
       <c r="M136" s="256" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="137" spans="13:13" ht="15.95" thickBot="1">
+    <row r="137" spans="13:13" ht="15.75" thickBot="1">
       <c r="M137" s="256" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="138" spans="13:13" ht="15.95" thickBot="1">
+    <row r="138" spans="13:13" ht="15.75" thickBot="1">
       <c r="M138" s="256" t="s">
         <v>487</v>
       </c>

</xml_diff>